<commit_message>
optimise ETL process on the biggest question related Fact
</commit_message>
<xml_diff>
--- a/lab04/Queries.xlsx
+++ b/lab04/Queries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HD\lab04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF26F50-B5DF-4132-9ABC-055BEEC03703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8811E58A-A827-4EAC-82B4-3FABAA93CE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="1" activeTab="8" xr2:uid="{0FE0208F-B594-46F3-BEE1-52AD3B7DC0C2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="1" activeTab="7" xr2:uid="{0FE0208F-B594-46F3-BEE1-52AD3B7DC0C2}"/>
   </bookViews>
   <sheets>
     <sheet name="3.3.1" sheetId="8" r:id="rId1"/>
@@ -27,17 +27,17 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="79" r:id="rId12"/>
-    <pivotCache cacheId="82" r:id="rId13"/>
-    <pivotCache cacheId="85" r:id="rId14"/>
-    <pivotCache cacheId="88" r:id="rId15"/>
-    <pivotCache cacheId="91" r:id="rId16"/>
-    <pivotCache cacheId="94" r:id="rId17"/>
-    <pivotCache cacheId="100" r:id="rId18"/>
-    <pivotCache cacheId="103" r:id="rId19"/>
-    <pivotCache cacheId="106" r:id="rId20"/>
-    <pivotCache cacheId="109" r:id="rId21"/>
-    <pivotCache cacheId="112" r:id="rId22"/>
+    <pivotCache cacheId="244" r:id="rId12"/>
+    <pivotCache cacheId="247" r:id="rId13"/>
+    <pivotCache cacheId="250" r:id="rId14"/>
+    <pivotCache cacheId="253" r:id="rId15"/>
+    <pivotCache cacheId="256" r:id="rId16"/>
+    <pivotCache cacheId="259" r:id="rId17"/>
+    <pivotCache cacheId="262" r:id="rId18"/>
+    <pivotCache cacheId="265" r:id="rId19"/>
+    <pivotCache cacheId="268" r:id="rId20"/>
+    <pivotCache cacheId="271" r:id="rId21"/>
+    <pivotCache cacheId="274" r:id="rId22"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="91">
   <si>
     <t>Średni czas oczekiwania na egzamin</t>
   </si>
@@ -231,9 +231,6 @@
     <t>Co oznacza znak 'Koniec autostrady'?</t>
   </si>
   <si>
-    <t>Co oznacza znak 'Koniec ograniczenia prędkości'?</t>
-  </si>
-  <si>
     <t>Co oznacza znak 'Uwaga, dzieci'?</t>
   </si>
   <si>
@@ -255,9 +252,6 @@
     <t>Co oznacza znak 'Znak ostrzegawczy' z symbolem skrzyżowania?</t>
   </si>
   <si>
-    <t>Czy można wyprzedzać pojazd na przejściu dla pieszych?</t>
-  </si>
-  <si>
     <t>Jakie jest dopuszczalne ciśnienie w oponach?</t>
   </si>
   <si>
@@ -273,9 +267,6 @@
     <t>Kiedy można używać klaksonu?</t>
   </si>
   <si>
-    <t>Kiedy należy używać pasów bezpieczeństwa?</t>
-  </si>
-  <si>
     <t>Kiedy należy używać świateł przeciwmgielnych?</t>
   </si>
   <si>
@@ -309,36 +300,18 @@
     <t>97030663488</t>
   </si>
   <si>
-    <t>Co oznacza znak 'Droga z pierwszeństwem'?</t>
-  </si>
-  <si>
-    <t>Czy można wyprzedzać na skrzyżowaniu?</t>
-  </si>
-  <si>
-    <t>Jakie jest maksymalne dopuszczalne stężenie alkoholu we krwi kierowcy w Polsce?</t>
-  </si>
-  <si>
     <t>Jakie jest minimalne ciśnienie w oponach?</t>
   </si>
   <si>
     <t>Jakie są zasady używania świateł drogowych poza terenem zabudowanym?</t>
   </si>
   <si>
-    <t>Co należy zrobić w przypadku awarii na autostradzie?</t>
-  </si>
-  <si>
-    <t>Co należy zrobić, gdy widzimy znak 'Zakaz parkowania'?</t>
-  </si>
-  <si>
     <t>Co należy zrobić, gdy widzimy znak 'Zakaz wjazdu rowerów'?</t>
   </si>
   <si>
     <t>Co oznacza znak 'Droga dla pieszych'?</t>
   </si>
   <si>
-    <t>Co oznacza znak 'Droga dla rowerów'?</t>
-  </si>
-  <si>
     <t>Co oznacza znak ograniczenie prędkości?</t>
   </si>
   <si>
@@ -348,9 +321,6 @@
     <t>Co oznacza znak 'Zakaz wjazdu motocykli'?</t>
   </si>
   <si>
-    <t>Co oznacza znak 'Zakaz wjazdu rowerów'?</t>
-  </si>
-  <si>
     <t>Co oznacza znak 'Zakaz wjazdu samochodów ciężarowych'?</t>
   </si>
   <si>
@@ -363,9 +333,6 @@
     <t>Czy można prowadzić pojazd bez ubezpieczenia?</t>
   </si>
   <si>
-    <t>Jakie jest minimalne ogumienie dozwolone na samochodzie osobowym?</t>
-  </si>
-  <si>
     <t>Co należy zrobić, gdy widzimy pojazd uprzywilejowany?</t>
   </si>
   <si>
@@ -384,12 +351,6 @@
     <t>Czy można korzystać z telefonu podczas prowadzenia pojazdu?</t>
   </si>
   <si>
-    <t>Jakie jest ograniczenie prędkości na autostradzie?</t>
-  </si>
-  <si>
-    <t>Jakie jest ograniczenie prędkości w terenie zabudowanym?</t>
-  </si>
-  <si>
     <t>Jakie jest pierwszeństwo na rondzie?</t>
   </si>
   <si>
@@ -397,9 +358,6 @@
   </si>
   <si>
     <t>Jakie są zasady używania świateł mijania w nocy?</t>
-  </si>
-  <si>
-    <t>Jakie są zasady używania świateł mijania?</t>
   </si>
   <si>
     <t>Jakie są zasady używania świateł przeciwmgielnych?</t>
@@ -976,61 +934,43 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45618.912822685183" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{D23C14AE-DFF4-46F3-8A87-861EEDD53DFD}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45636.828921759261" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{EDAA29B6-B94C-4D0A-8196-521B5732F82D}">
   <cacheSource type="external" connectionId="1"/>
-  <cacheFields count="6">
-    <cacheField name="[Measures].[Liczba egzaminów]" caption="Liczba egzaminów" numFmtId="0" hierarchy="34" level="32767"/>
-    <cacheField name="[Zajetosc Terminu Egzaminu].[Zajetosc Terminu].[Zajetosc Terminu]" caption="Zajetosc Terminu" numFmtId="0" hierarchy="28" level="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-    <cacheField name="[Data].[Hierarchy].[Rok]" caption="Rok" numFmtId="0" hierarchy="5" level="1">
-      <sharedItems count="1">
-        <s v="[Data].[Hierarchy].[Rok].&amp;[2021]" c="2021"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Data].[Hierarchy].[Miesiac]" caption="Miesiac" numFmtId="0" hierarchy="5" level="2" mappingCount="1">
-      <sharedItems count="5">
-        <s v="[Data].[Hierarchy].[Rok].&amp;[2021].&amp;[Styczeń]" c="Styczeń"/>
-        <s v="[Data].[Hierarchy].[Rok].&amp;[2021].&amp;[Luty]" c="Luty"/>
-        <s v="[Data].[Hierarchy].[Rok].&amp;[2021].&amp;[Marzec]" c="Marzec"/>
-        <s v="[Data].[Hierarchy].[Rok].&amp;[2021].&amp;[Kwiecień]" c="Kwiecień"/>
-        <s v="[Data].[Hierarchy].[Rok].&amp;[2021].&amp;[Maj]" c="Maj"/>
-      </sharedItems>
-      <mpMap v="5"/>
-    </cacheField>
-    <cacheField name="[Data].[Hierarchy].[Data]" caption="Data" numFmtId="0" hierarchy="5" level="3">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-    <cacheField name="[Data].[Hierarchy].[Miesiac].[Numer Miesiaca]" caption="Numer Miesiaca" propertyName="Numer Miesiaca" numFmtId="0" hierarchy="5" level="2" memberPropertyField="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5" count="5">
-        <n v="1"/>
-        <n v="2"/>
-        <n v="3"/>
-        <n v="4"/>
-        <n v="5"/>
+  <cacheFields count="2">
+    <cacheField name="[Measures].[Liczba pytań]" caption="Liczba pytań" numFmtId="0" hierarchy="40" level="32767"/>
+    <cacheField name="[Egzaminator].[Pesel].[Pesel]" caption="Pesel" numFmtId="0" hierarchy="11" level="1">
+      <sharedItems count="10">
+        <s v="[Egzaminator].[Pesel].&amp;[14040288601]" c="14040288601"/>
+        <s v="[Egzaminator].[Pesel].&amp;[16012395393]" c="16012395393"/>
+        <s v="[Egzaminator].[Pesel].&amp;[16042143005]" c="16042143005"/>
+        <s v="[Egzaminator].[Pesel].&amp;[19021381580]" c="19021381580"/>
+        <s v="[Egzaminator].[Pesel].&amp;[23250762146]" c="23250762146"/>
+        <s v="[Egzaminator].[Pesel].&amp;[46011838544]" c="46011838544"/>
+        <s v="[Egzaminator].[Pesel].&amp;[49010714778]" c="49010714778"/>
+        <s v="[Egzaminator].[Pesel].&amp;[57050594043]" c="57050594043"/>
+        <s v="[Egzaminator].[Pesel].&amp;[88080744315]" c="88080744315"/>
+        <s v="[Egzaminator].[Pesel].&amp;[97030663488]" c="97030663488"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
-  <cacheHierarchies count="45">
+  <cacheHierarchies count="53">
     <cacheHierarchy uniqueName="[Czas].[Godzina]" caption="Godzina" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Godzina].[All]" allUniqueName="[Czas].[Godzina].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[ID Czasu]" caption="ID Czasu" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Czas].[ID Czasu].[All]" allUniqueName="[Czas].[ID Czasu].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[Minuty]" caption="Minuty" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Minuty].[All]" allUniqueName="[Czas].[Minuty].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[Data]" caption="Data" attribute="1" time="1" defaultMemberUniqueName="[Data].[Data].[All]" allUniqueName="[Data].[Data].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[Dzien Tygodnia]" caption="Dzien Tygodnia" attribute="1" time="1" defaultMemberUniqueName="[Data].[Dzien Tygodnia].[All]" allUniqueName="[Data].[Dzien Tygodnia].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data].[Hierarchy]" caption="Hierarchy" time="1" defaultMemberUniqueName="[Data].[Hierarchy].[All]" allUniqueName="[Data].[Hierarchy].[All]" dimensionUniqueName="[Data]" displayFolder="" count="4" unbalanced="0">
-      <fieldsUsage count="4">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="2"/>
-        <fieldUsage x="3"/>
-        <fieldUsage x="4"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Data].[Hierarchy]" caption="Hierarchy" time="1" defaultMemberUniqueName="[Data].[Hierarchy].[All]" allUniqueName="[Data].[Hierarchy].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[ID Daty]" caption="ID Daty" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data].[ID Daty].[All]" allUniqueName="[Data].[ID Daty].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[Miesiac]" caption="Miesiac" attribute="1" time="1" defaultMemberUniqueName="[Data].[Miesiac].[All]" allUniqueName="[Data].[Miesiac].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[Rok]" caption="Rok" attribute="1" time="1" defaultMemberUniqueName="[Data].[Rok].[All]" allUniqueName="[Data].[Rok].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Egzaminator].[ID Egzaminatora]" caption="ID Egzaminatora" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Egzaminator].[ID Egzaminatora].[All]" allUniqueName="[Egzaminator].[ID Egzaminatora].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Egzaminator].[Imie I Nazwisko]" caption="Imie I Nazwisko" attribute="1" defaultMemberUniqueName="[Egzaminator].[Imie I Nazwisko].[All]" allUniqueName="[Egzaminator].[Imie I Nazwisko].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Egzaminator].[Pesel]" caption="Pesel" attribute="1" defaultMemberUniqueName="[Egzaminator].[Pesel].[All]" allUniqueName="[Egzaminator].[Pesel].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Egzaminator].[Pesel]" caption="Pesel" attribute="1" defaultMemberUniqueName="[Egzaminator].[Pesel].[All]" allUniqueName="[Egzaminator].[Pesel].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Kandydat].[ID Kandydata]" caption="ID Kandydata" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Kandydat].[ID Kandydata].[All]" allUniqueName="[Kandydat].[ID Kandydata].[All]" dimensionUniqueName="[Kandydat]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Kandydat].[PKK]" caption="PKK" attribute="1" defaultMemberUniqueName="[Kandydat].[PKK].[All]" allUniqueName="[Kandydat].[PKK].[All]" dimensionUniqueName="[Kandydat]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Pytanie].[ID Pytania]" caption="ID Pytania" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Pytanie].[ID Pytania].[All]" allUniqueName="[Pytanie].[ID Pytania].[All]" dimensionUniqueName="[Pytanie]" displayFolder="" count="0" unbalanced="0"/>
@@ -1047,34 +987,40 @@
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Terminu Egzaminu]" caption="ID Terminu Egzaminu" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Terminu Egzaminu].[All]" allUniqueName="[Termin Egzaminu].[ID Terminu Egzaminu].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[Numer Sali Egzaminacyjnej]" caption="Numer Sali Egzaminacyjnej" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].[All]" allUniqueName="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Zajetosc Terminu Egzaminu].[ID Zajetosci Terminu Egzaminu]" caption="ID Zajetosci Terminu Egzaminu" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Zajetosc Terminu Egzaminu].[ID Zajetosci Terminu Egzaminu].[All]" allUniqueName="[Zajetosc Terminu Egzaminu].[ID Zajetosci Terminu Egzaminu].[All]" dimensionUniqueName="[Zajetosc Terminu Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Zajetosc Terminu Egzaminu].[Zajetosc Terminu]" caption="Zajetosc Terminu" attribute="1" defaultMemberUniqueName="[Zajetosc Terminu Egzaminu].[Zajetosc Terminu].[All]" allUniqueName="[Zajetosc Terminu Egzaminu].[Zajetosc Terminu].[All]" dimensionUniqueName="[Zajetosc Terminu Egzaminu]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Zajetosc Terminu Egzaminu].[Zajetosc Terminu]" caption="Zajetosc Terminu" attribute="1" defaultMemberUniqueName="[Zajetosc Terminu Egzaminu].[Zajetosc Terminu].[All]" allUniqueName="[Zajetosc Terminu Egzaminu].[Zajetosc Terminu].[All]" dimensionUniqueName="[Zajetosc Terminu Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba rezerwacji na termin]" caption="Liczba rezerwacji na termin" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączny czas oczekiwania na egzamin]" caption="Łączny czas oczekiwania na egzamin" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba rezerwacji]" caption="Liczba rezerwacji" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba różnych dni wśród terminów rezerwacji]" caption="Liczba różnych dni wśród terminów rezerwacji" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu 1" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba różnych kandydatów wśród terminów rezerwacji]" caption="Liczba różnych kandydatów wśród terminów rezerwacji" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu 2" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba egzaminów]" caption="Liczba egzaminów" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0" oneField="1">
-      <fieldsUsage count="1">
-        <fieldUsage x="0"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Liczba egzaminów]" caption="Liczba egzaminów" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba uczestników]" caption="Łączna liczba uczestników" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba rezerwacji]" caption="Łączna liczba rezerwacji" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba skarg]" caption="Liczba skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba powiązanych incydentów]" caption="Liczba powiązanych incydentów" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba kandydatów którzy złożyli skargi]" caption="Liczba kandydatów którzy złożyli skargi" measure="1" displayFolder="" measureGroup="Zlozenie Skargi 1" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba pytań]" caption="Liczba pytań" measure="1" displayFolder="" measureGroup="Odpowiedzenie Na Pytanie Podczas Egzaminu Ze Skarga" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Liczba pytań]" caption="Liczba pytań" measure="1" displayFolder="" measureGroup="Odpowiedzenie Na Pytanie Podczas Egzaminu Ze Skarga" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji]" caption="Średnia liczba rezerwacji" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Średni czas oczekiwania na egzamin]" caption="Średni czas oczekiwania na egzamin" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji na kandydata]" caption="Średnia liczba rezerwacji na kandydata" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba kandydatów nieobecnych]" caption="Łączna liczba kandydatów nieobecnych" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Value]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Goal)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Status)" measure="1" iconSet="8" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Trend)" measure="1" iconSet="5" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Liczby Skarg Value]" caption="Zmniejszenie Liczby Skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Goal]" caption="Zmniejszenie Liczby Skarg (Goal)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Status]" caption="Zmniejszenie Liczby Skarg (Status)" measure="1" iconSet="8" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Trend]" caption="Zmniejszenie Liczby Skarg (Trend)" measure="1" iconSet="5" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
   </cacheHierarchies>
-  <kpis count="0"/>
+  <kpis count="2">
+    <kpi uniqueName="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" displayFolder="" measureGroup="Zarezerwowanie Terminu" parent="" value="[Measures].[Średni czas oczekiwania na egzamin]" goal="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" status="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" trend="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" weight=""/>
+    <kpi uniqueName="Zmniejszenie Liczby Skarg" caption="Zmniejszenie Liczby Skarg" displayFolder="" measureGroup="Zlozenie Skargi" parent="" value="[Measures].[Liczba skarg]" goal="[Measures].[Zmniejszenie Liczby Skarg Goal]" status="[Measures].[Zmniejszenie Liczby Skarg Status]" trend="[Measures].[Zmniejszenie Liczby Skarg Trend]" weight=""/>
+  </kpis>
   <dimensions count="9">
     <dimension name="Czas" uniqueName="[Czas]" caption="Czas"/>
     <dimension name="Data" uniqueName="[Data]" caption="Data"/>
@@ -1146,36 +1092,18 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45618.912828009263" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{37400404-E3DB-4AA7-9B37-483ECC7E0774}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45636.828954745368" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{1733CCD2-B9F2-4756-8539-214B3CA0E949}">
   <cacheSource type="external" connectionId="1"/>
-  <cacheFields count="4">
-    <cacheField name="[Measures].[Liczba skarg]" caption="Liczba skarg" numFmtId="0" hierarchy="37" level="32767"/>
-    <cacheField name="[Data].[Rok].[Rok]" caption="Rok" numFmtId="0" hierarchy="8" level="1">
-      <sharedItems count="1">
-        <s v="[Data].[Rok].&amp;[2021]" c="2021"/>
-      </sharedItems>
+  <cacheFields count="3">
+    <cacheField name="[Measures].[Liczba kandydatów którzy złożyli skargi]" caption="Liczba kandydatów którzy złożyli skargi" numFmtId="0" hierarchy="39" level="32767"/>
+    <cacheField name="[Skarga].[Typ Skargi].[Typ Skargi]" caption="Typ Skargi" numFmtId="0" hierarchy="21" level="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
     </cacheField>
-    <cacheField name="[Data].[Miesiac].[Miesiac]" caption="Miesiac" numFmtId="0" hierarchy="7" level="1" mappingCount="1">
-      <sharedItems count="5">
-        <s v="[Data].[Miesiac].&amp;[Styczeń]" c="Styczeń"/>
-        <s v="[Data].[Miesiac].&amp;[Luty]" c="Luty"/>
-        <s v="[Data].[Miesiac].&amp;[Marzec]" c="Marzec"/>
-        <s v="[Data].[Miesiac].&amp;[Kwiecień]" c="Kwiecień"/>
-        <s v="[Data].[Miesiac].&amp;[Maj]" c="Maj"/>
-      </sharedItems>
-      <mpMap v="3"/>
-    </cacheField>
-    <cacheField name="[Data].[Miesiac].[Miesiac].[Numer Miesiaca]" caption="Numer Miesiaca" propertyName="Numer Miesiaca" numFmtId="0" hierarchy="7" level="1" memberPropertyField="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5" count="5">
-        <n v="1"/>
-        <n v="2"/>
-        <n v="3"/>
-        <n v="4"/>
-        <n v="5"/>
-      </sharedItems>
+    <cacheField name="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania]" caption="Czy Kandydat Odpowiedzial Na Wszystkie Pytania" numFmtId="0" hierarchy="17" level="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
     </cacheField>
   </cacheFields>
-  <cacheHierarchies count="45">
+  <cacheHierarchies count="53">
     <cacheHierarchy uniqueName="[Czas].[Godzina]" caption="Godzina" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Godzina].[All]" allUniqueName="[Czas].[Godzina].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[ID Czasu]" caption="ID Czasu" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Czas].[ID Czasu].[All]" allUniqueName="[Czas].[ID Czasu].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[Minuty]" caption="Minuty" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Minuty].[All]" allUniqueName="[Czas].[Minuty].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
@@ -1183,18 +1111,8 @@
     <cacheHierarchy uniqueName="[Data].[Dzien Tygodnia]" caption="Dzien Tygodnia" attribute="1" time="1" defaultMemberUniqueName="[Data].[Dzien Tygodnia].[All]" allUniqueName="[Data].[Dzien Tygodnia].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[Hierarchy]" caption="Hierarchy" time="1" defaultMemberUniqueName="[Data].[Hierarchy].[All]" allUniqueName="[Data].[Hierarchy].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[ID Daty]" caption="ID Daty" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data].[ID Daty].[All]" allUniqueName="[Data].[ID Daty].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data].[Miesiac]" caption="Miesiac" attribute="1" time="1" defaultMemberUniqueName="[Data].[Miesiac].[All]" allUniqueName="[Data].[Miesiac].[All]" dimensionUniqueName="[Data]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="2"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Data].[Rok]" caption="Rok" attribute="1" time="1" defaultMemberUniqueName="[Data].[Rok].[All]" allUniqueName="[Data].[Rok].[All]" dimensionUniqueName="[Data]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Data].[Miesiac]" caption="Miesiac" attribute="1" time="1" defaultMemberUniqueName="[Data].[Miesiac].[All]" allUniqueName="[Data].[Miesiac].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data].[Rok]" caption="Rok" attribute="1" time="1" defaultMemberUniqueName="[Data].[Rok].[All]" allUniqueName="[Data].[Rok].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Egzaminator].[ID Egzaminatora]" caption="ID Egzaminatora" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Egzaminator].[ID Egzaminatora].[All]" allUniqueName="[Egzaminator].[ID Egzaminatora].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Egzaminator].[Imie I Nazwisko]" caption="Imie I Nazwisko" attribute="1" defaultMemberUniqueName="[Egzaminator].[Imie I Nazwisko].[All]" allUniqueName="[Egzaminator].[Imie I Nazwisko].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Egzaminator].[Pesel]" caption="Pesel" attribute="1" defaultMemberUniqueName="[Egzaminator].[Pesel].[All]" allUniqueName="[Egzaminator].[Pesel].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
@@ -1203,11 +1121,21 @@
     <cacheHierarchy uniqueName="[Pytanie].[ID Pytania]" caption="ID Pytania" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Pytanie].[ID Pytania].[All]" allUniqueName="[Pytanie].[ID Pytania].[All]" dimensionUniqueName="[Pytanie]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Pytanie].[Tresc]" caption="Tresc" attribute="1" defaultMemberUniqueName="[Pytanie].[Tresc].[All]" allUniqueName="[Pytanie].[Tresc].[All]" dimensionUniqueName="[Pytanie]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty]" caption="Czy Istnieja Powiazane Incydenty" attribute="1" defaultMemberUniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty].[All]" allUniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania]" caption="Czy Kandydat Odpowiedzial Na Wszystkie Pytania" attribute="1" defaultMemberUniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania].[All]" allUniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania]" caption="Czy Kandydat Odpowiedzial Na Wszystkie Pytania" attribute="1" defaultMemberUniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania].[All]" allUniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="2"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Skarga].[Hierarchy]" caption="Hierarchy" defaultMemberUniqueName="[Skarga].[Hierarchy].[All]" allUniqueName="[Skarga].[Hierarchy].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[ID Skargi]" caption="ID Skargi" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Skarga].[ID Skargi].[All]" allUniqueName="[Skarga].[ID Skargi].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[Typ Egzaminu]" caption="Typ Egzaminu" attribute="1" defaultMemberUniqueName="[Skarga].[Typ Egzaminu].[All]" allUniqueName="[Skarga].[Typ Egzaminu].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Skarga].[Typ Skargi]" caption="Typ Skargi" attribute="1" defaultMemberUniqueName="[Skarga].[Typ Skargi].[All]" allUniqueName="[Skarga].[Typ Skargi].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Skarga].[Typ Skargi]" caption="Typ Skargi" attribute="1" defaultMemberUniqueName="[Skarga].[Typ Skargi].[All]" allUniqueName="[Skarga].[Typ Skargi].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Czasu]" caption="ID Czasu" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Czasu].[All]" allUniqueName="[Termin Egzaminu].[ID Czasu].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Daty]" caption="ID Daty" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Daty].[All]" allUniqueName="[Termin Egzaminu].[ID Daty].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Egzaminatora]" caption="ID Egzaminatora" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Egzaminatora].[All]" allUniqueName="[Termin Egzaminu].[ID Egzaminatora].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
@@ -1223,20 +1151,31 @@
     <cacheHierarchy uniqueName="[Measures].[Liczba egzaminów]" caption="Liczba egzaminów" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba uczestników]" caption="Łączna liczba uczestników" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba rezerwacji]" caption="Łączna liczba rezerwacji" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba skarg]" caption="Liczba skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" oneField="1">
+    <cacheHierarchy uniqueName="[Measures].[Liczba skarg]" caption="Liczba skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Liczba powiązanych incydentów]" caption="Liczba powiązanych incydentów" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Liczba kandydatów którzy złożyli skargi]" caption="Liczba kandydatów którzy złożyli skargi" measure="1" displayFolder="" measureGroup="Zlozenie Skargi 1" count="0" oneField="1">
       <fieldsUsage count="1">
         <fieldUsage x="0"/>
       </fieldsUsage>
     </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Measures].[Liczba powiązanych incydentów]" caption="Liczba powiązanych incydentów" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba kandydatów którzy złożyli skargi]" caption="Liczba kandydatów którzy złożyli skargi" measure="1" displayFolder="" measureGroup="Zlozenie Skargi 1" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba pytań]" caption="Liczba pytań" measure="1" displayFolder="" measureGroup="Odpowiedzenie Na Pytanie Podczas Egzaminu Ze Skarga" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji]" caption="Średnia liczba rezerwacji" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Średni czas oczekiwania na egzamin]" caption="Średni czas oczekiwania na egzamin" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji na kandydata]" caption="Średnia liczba rezerwacji na kandydata" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba kandydatów nieobecnych]" caption="Łączna liczba kandydatów nieobecnych" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Value]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Goal)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Status)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Trend)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Liczby Skarg Value]" caption="Zmniejszenie Liczby Skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Goal]" caption="Zmniejszenie Liczby Skarg (Goal)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Status]" caption="Zmniejszenie Liczby Skarg (Status)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Trend]" caption="Zmniejszenie Liczby Skarg (Trend)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
   </cacheHierarchies>
-  <kpis count="0"/>
+  <kpis count="2">
+    <kpi uniqueName="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" displayFolder="" measureGroup="Zarezerwowanie Terminu" parent="" value="[Measures].[Średni czas oczekiwania na egzamin]" goal="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" status="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" trend="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" weight=""/>
+    <kpi uniqueName="Zmniejszenie Liczby Skarg" caption="Zmniejszenie Liczby Skarg" displayFolder="" measureGroup="Zlozenie Skargi" parent="" value="[Measures].[Liczba skarg]" goal="[Measures].[Zmniejszenie Liczby Skarg Goal]" status="[Measures].[Zmniejszenie Liczby Skarg Status]" trend="[Measures].[Zmniejszenie Liczby Skarg Trend]" weight=""/>
+  </kpis>
   <dimensions count="9">
     <dimension name="Czas" uniqueName="[Czas]" caption="Czas"/>
     <dimension name="Data" uniqueName="[Data]" caption="Data"/>
@@ -1308,43 +1247,61 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45618.912944560187" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{EDAA29B6-B94C-4D0A-8196-521B5732F82D}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45636.82895787037" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{D23C14AE-DFF4-46F3-8A87-861EEDD53DFD}">
   <cacheSource type="external" connectionId="1"/>
-  <cacheFields count="2">
-    <cacheField name="[Measures].[Liczba pytań]" caption="Liczba pytań" numFmtId="0" hierarchy="40" level="32767"/>
-    <cacheField name="[Egzaminator].[Pesel].[Pesel]" caption="Pesel" numFmtId="0" hierarchy="11" level="1">
-      <sharedItems count="10">
-        <s v="[Egzaminator].[Pesel].&amp;[14040288601]" c="14040288601"/>
-        <s v="[Egzaminator].[Pesel].&amp;[16012395393]" c="16012395393"/>
-        <s v="[Egzaminator].[Pesel].&amp;[16042143005]" c="16042143005"/>
-        <s v="[Egzaminator].[Pesel].&amp;[19021381580]" c="19021381580"/>
-        <s v="[Egzaminator].[Pesel].&amp;[23250762146]" c="23250762146"/>
-        <s v="[Egzaminator].[Pesel].&amp;[46011838544]" c="46011838544"/>
-        <s v="[Egzaminator].[Pesel].&amp;[49010714778]" c="49010714778"/>
-        <s v="[Egzaminator].[Pesel].&amp;[57050594043]" c="57050594043"/>
-        <s v="[Egzaminator].[Pesel].&amp;[88080744315]" c="88080744315"/>
-        <s v="[Egzaminator].[Pesel].&amp;[97030663488]" c="97030663488"/>
+  <cacheFields count="6">
+    <cacheField name="[Measures].[Liczba egzaminów]" caption="Liczba egzaminów" numFmtId="0" hierarchy="34" level="32767"/>
+    <cacheField name="[Zajetosc Terminu Egzaminu].[Zajetosc Terminu].[Zajetosc Terminu]" caption="Zajetosc Terminu" numFmtId="0" hierarchy="28" level="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Data].[Hierarchy].[Rok]" caption="Rok" numFmtId="0" hierarchy="5" level="1">
+      <sharedItems count="1">
+        <s v="[Data].[Hierarchy].[Rok].&amp;[2021]" c="2021"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Data].[Hierarchy].[Miesiac]" caption="Miesiac" numFmtId="0" hierarchy="5" level="2" mappingCount="1">
+      <sharedItems count="5">
+        <s v="[Data].[Hierarchy].[Rok].&amp;[2021].&amp;[Styczeń]" c="Styczeń"/>
+        <s v="[Data].[Hierarchy].[Rok].&amp;[2021].&amp;[Luty]" c="Luty"/>
+        <s v="[Data].[Hierarchy].[Rok].&amp;[2021].&amp;[Marzec]" c="Marzec"/>
+        <s v="[Data].[Hierarchy].[Rok].&amp;[2021].&amp;[Kwiecień]" c="Kwiecień"/>
+        <s v="[Data].[Hierarchy].[Rok].&amp;[2021].&amp;[Maj]" c="Maj"/>
+      </sharedItems>
+      <mpMap v="5"/>
+    </cacheField>
+    <cacheField name="[Data].[Hierarchy].[Data]" caption="Data" numFmtId="0" hierarchy="5" level="3">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Data].[Hierarchy].[Miesiac].[Numer Miesiaca]" caption="Numer Miesiaca" propertyName="Numer Miesiaca" numFmtId="0" hierarchy="5" level="2" memberPropertyField="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5" count="5">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="3"/>
+        <n v="4"/>
+        <n v="5"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
-  <cacheHierarchies count="45">
+  <cacheHierarchies count="53">
     <cacheHierarchy uniqueName="[Czas].[Godzina]" caption="Godzina" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Godzina].[All]" allUniqueName="[Czas].[Godzina].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[ID Czasu]" caption="ID Czasu" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Czas].[ID Czasu].[All]" allUniqueName="[Czas].[ID Czasu].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[Minuty]" caption="Minuty" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Minuty].[All]" allUniqueName="[Czas].[Minuty].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[Data]" caption="Data" attribute="1" time="1" defaultMemberUniqueName="[Data].[Data].[All]" allUniqueName="[Data].[Data].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[Dzien Tygodnia]" caption="Dzien Tygodnia" attribute="1" time="1" defaultMemberUniqueName="[Data].[Dzien Tygodnia].[All]" allUniqueName="[Data].[Dzien Tygodnia].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data].[Hierarchy]" caption="Hierarchy" time="1" defaultMemberUniqueName="[Data].[Hierarchy].[All]" allUniqueName="[Data].[Hierarchy].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data].[Hierarchy]" caption="Hierarchy" time="1" defaultMemberUniqueName="[Data].[Hierarchy].[All]" allUniqueName="[Data].[Hierarchy].[All]" dimensionUniqueName="[Data]" displayFolder="" count="4" unbalanced="0">
+      <fieldsUsage count="4">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="2"/>
+        <fieldUsage x="3"/>
+        <fieldUsage x="4"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Data].[ID Daty]" caption="ID Daty" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data].[ID Daty].[All]" allUniqueName="[Data].[ID Daty].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[Miesiac]" caption="Miesiac" attribute="1" time="1" defaultMemberUniqueName="[Data].[Miesiac].[All]" allUniqueName="[Data].[Miesiac].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[Rok]" caption="Rok" attribute="1" time="1" defaultMemberUniqueName="[Data].[Rok].[All]" allUniqueName="[Data].[Rok].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Egzaminator].[ID Egzaminatora]" caption="ID Egzaminatora" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Egzaminator].[ID Egzaminatora].[All]" allUniqueName="[Egzaminator].[ID Egzaminatora].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Egzaminator].[Imie I Nazwisko]" caption="Imie I Nazwisko" attribute="1" defaultMemberUniqueName="[Egzaminator].[Imie I Nazwisko].[All]" allUniqueName="[Egzaminator].[Imie I Nazwisko].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="2" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Egzaminator].[Pesel]" caption="Pesel" attribute="1" defaultMemberUniqueName="[Egzaminator].[Pesel].[All]" allUniqueName="[Egzaminator].[Pesel].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Egzaminator].[Imie I Nazwisko]" caption="Imie I Nazwisko" attribute="1" defaultMemberUniqueName="[Egzaminator].[Imie I Nazwisko].[All]" allUniqueName="[Egzaminator].[Imie I Nazwisko].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Egzaminator].[Pesel]" caption="Pesel" attribute="1" defaultMemberUniqueName="[Egzaminator].[Pesel].[All]" allUniqueName="[Egzaminator].[Pesel].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Kandydat].[ID Kandydata]" caption="ID Kandydata" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Kandydat].[ID Kandydata].[All]" allUniqueName="[Kandydat].[ID Kandydata].[All]" dimensionUniqueName="[Kandydat]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Kandydat].[PKK]" caption="PKK" attribute="1" defaultMemberUniqueName="[Kandydat].[PKK].[All]" allUniqueName="[Kandydat].[PKK].[All]" dimensionUniqueName="[Kandydat]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Pytanie].[ID Pytania]" caption="ID Pytania" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Pytanie].[ID Pytania].[All]" allUniqueName="[Pytanie].[ID Pytania].[All]" dimensionUniqueName="[Pytanie]" displayFolder="" count="0" unbalanced="0"/>
@@ -1361,29 +1318,45 @@
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Terminu Egzaminu]" caption="ID Terminu Egzaminu" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Terminu Egzaminu].[All]" allUniqueName="[Termin Egzaminu].[ID Terminu Egzaminu].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[Numer Sali Egzaminacyjnej]" caption="Numer Sali Egzaminacyjnej" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].[All]" allUniqueName="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Zajetosc Terminu Egzaminu].[ID Zajetosci Terminu Egzaminu]" caption="ID Zajetosci Terminu Egzaminu" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Zajetosc Terminu Egzaminu].[ID Zajetosci Terminu Egzaminu].[All]" allUniqueName="[Zajetosc Terminu Egzaminu].[ID Zajetosci Terminu Egzaminu].[All]" dimensionUniqueName="[Zajetosc Terminu Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Zajetosc Terminu Egzaminu].[Zajetosc Terminu]" caption="Zajetosc Terminu" attribute="1" defaultMemberUniqueName="[Zajetosc Terminu Egzaminu].[Zajetosc Terminu].[All]" allUniqueName="[Zajetosc Terminu Egzaminu].[Zajetosc Terminu].[All]" dimensionUniqueName="[Zajetosc Terminu Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Zajetosc Terminu Egzaminu].[Zajetosc Terminu]" caption="Zajetosc Terminu" attribute="1" defaultMemberUniqueName="[Zajetosc Terminu Egzaminu].[Zajetosc Terminu].[All]" allUniqueName="[Zajetosc Terminu Egzaminu].[Zajetosc Terminu].[All]" dimensionUniqueName="[Zajetosc Terminu Egzaminu]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[Liczba rezerwacji na termin]" caption="Liczba rezerwacji na termin" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączny czas oczekiwania na egzamin]" caption="Łączny czas oczekiwania na egzamin" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba rezerwacji]" caption="Liczba rezerwacji" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba różnych dni wśród terminów rezerwacji]" caption="Liczba różnych dni wśród terminów rezerwacji" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu 1" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba różnych kandydatów wśród terminów rezerwacji]" caption="Liczba różnych kandydatów wśród terminów rezerwacji" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu 2" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba egzaminów]" caption="Liczba egzaminów" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Liczba egzaminów]" caption="Liczba egzaminów" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba uczestników]" caption="Łączna liczba uczestników" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba rezerwacji]" caption="Łączna liczba rezerwacji" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba skarg]" caption="Liczba skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba powiązanych incydentów]" caption="Liczba powiązanych incydentów" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba kandydatów którzy złożyli skargi]" caption="Liczba kandydatów którzy złożyli skargi" measure="1" displayFolder="" measureGroup="Zlozenie Skargi 1" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba pytań]" caption="Liczba pytań" measure="1" displayFolder="" measureGroup="Odpowiedzenie Na Pytanie Podczas Egzaminu Ze Skarga" count="0" oneField="1">
-      <fieldsUsage count="1">
-        <fieldUsage x="0"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Liczba pytań]" caption="Liczba pytań" measure="1" displayFolder="" measureGroup="Odpowiedzenie Na Pytanie Podczas Egzaminu Ze Skarga" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji]" caption="Średnia liczba rezerwacji" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Średni czas oczekiwania na egzamin]" caption="Średni czas oczekiwania na egzamin" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji na kandydata]" caption="Średnia liczba rezerwacji na kandydata" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba kandydatów nieobecnych]" caption="Łączna liczba kandydatów nieobecnych" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Value]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Goal)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Status)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Trend)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Liczby Skarg Value]" caption="Zmniejszenie Liczby Skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Goal]" caption="Zmniejszenie Liczby Skarg (Goal)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Status]" caption="Zmniejszenie Liczby Skarg (Status)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Trend]" caption="Zmniejszenie Liczby Skarg (Trend)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
   </cacheHierarchies>
-  <kpis count="0"/>
+  <kpis count="2">
+    <kpi uniqueName="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" displayFolder="" measureGroup="Zarezerwowanie Terminu" parent="" value="[Measures].[Średni czas oczekiwania na egzamin]" goal="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" status="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" trend="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" weight=""/>
+    <kpi uniqueName="Zmniejszenie Liczby Skarg" caption="Zmniejszenie Liczby Skarg" displayFolder="" measureGroup="Zlozenie Skargi" parent="" value="[Measures].[Liczba skarg]" goal="[Measures].[Zmniejszenie Liczby Skarg Goal]" status="[Measures].[Zmniejszenie Liczby Skarg Status]" trend="[Measures].[Zmniejszenie Liczby Skarg Trend]" weight=""/>
+  </kpis>
   <dimensions count="9">
     <dimension name="Czas" uniqueName="[Czas]" caption="Czas"/>
     <dimension name="Data" uniqueName="[Data]" caption="Data"/>
@@ -1455,18 +1428,32 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45618.912822916667" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{1733CCD2-B9F2-4756-8539-214B3CA0E949}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45636.828926736111" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{37400404-E3DB-4AA7-9B37-483ECC7E0774}">
   <cacheSource type="external" connectionId="1"/>
-  <cacheFields count="3">
-    <cacheField name="[Measures].[Liczba kandydatów którzy złożyli skargi]" caption="Liczba kandydatów którzy złożyli skargi" numFmtId="0" hierarchy="39" level="32767"/>
-    <cacheField name="[Skarga].[Typ Skargi].[Typ Skargi]" caption="Typ Skargi" numFmtId="0" hierarchy="21" level="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+  <cacheFields count="4">
+    <cacheField name="[Measures].[Liczba skarg]" caption="Liczba skarg" numFmtId="0" hierarchy="37" level="32767"/>
+    <cacheField name="[Data].[Rok].[Rok]" caption="Rok" numFmtId="0" hierarchy="8" level="1">
+      <sharedItems count="1">
+        <s v="[Data].[Rok].&amp;[2021]" c="2021"/>
+      </sharedItems>
     </cacheField>
-    <cacheField name="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania]" caption="Czy Kandydat Odpowiedzial Na Wszystkie Pytania" numFmtId="0" hierarchy="17" level="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    <cacheField name="[Data].[Miesiac].[Miesiac]" caption="Miesiac" numFmtId="0" hierarchy="7" level="1" mappingCount="1">
+      <sharedItems count="3">
+        <s v="[Data].[Miesiac].&amp;[Marzec]" c="Marzec"/>
+        <s v="[Data].[Miesiac].&amp;[Kwiecień]" c="Kwiecień"/>
+        <s v="[Data].[Miesiac].&amp;[Maj]" c="Maj"/>
+      </sharedItems>
+      <mpMap v="3"/>
+    </cacheField>
+    <cacheField name="[Data].[Miesiac].[Miesiac].[Numer Miesiaca]" caption="Numer Miesiaca" propertyName="Numer Miesiaca" numFmtId="0" hierarchy="7" level="1" memberPropertyField="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="3" maxValue="5" count="3">
+        <n v="3"/>
+        <n v="4"/>
+        <n v="5"/>
+      </sharedItems>
     </cacheField>
   </cacheFields>
-  <cacheHierarchies count="45">
+  <cacheHierarchies count="53">
     <cacheHierarchy uniqueName="[Czas].[Godzina]" caption="Godzina" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Godzina].[All]" allUniqueName="[Czas].[Godzina].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[ID Czasu]" caption="ID Czasu" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Czas].[ID Czasu].[All]" allUniqueName="[Czas].[ID Czasu].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[Minuty]" caption="Minuty" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Minuty].[All]" allUniqueName="[Czas].[Minuty].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
@@ -1474,8 +1461,18 @@
     <cacheHierarchy uniqueName="[Data].[Dzien Tygodnia]" caption="Dzien Tygodnia" attribute="1" time="1" defaultMemberUniqueName="[Data].[Dzien Tygodnia].[All]" allUniqueName="[Data].[Dzien Tygodnia].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[Hierarchy]" caption="Hierarchy" time="1" defaultMemberUniqueName="[Data].[Hierarchy].[All]" allUniqueName="[Data].[Hierarchy].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[ID Daty]" caption="ID Daty" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data].[ID Daty].[All]" allUniqueName="[Data].[ID Daty].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data].[Miesiac]" caption="Miesiac" attribute="1" time="1" defaultMemberUniqueName="[Data].[Miesiac].[All]" allUniqueName="[Data].[Miesiac].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data].[Rok]" caption="Rok" attribute="1" time="1" defaultMemberUniqueName="[Data].[Rok].[All]" allUniqueName="[Data].[Rok].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data].[Miesiac]" caption="Miesiac" attribute="1" time="1" defaultMemberUniqueName="[Data].[Miesiac].[All]" allUniqueName="[Data].[Miesiac].[All]" dimensionUniqueName="[Data]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="2"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Data].[Rok]" caption="Rok" attribute="1" time="1" defaultMemberUniqueName="[Data].[Rok].[All]" allUniqueName="[Data].[Rok].[All]" dimensionUniqueName="[Data]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Egzaminator].[ID Egzaminatora]" caption="ID Egzaminatora" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Egzaminator].[ID Egzaminatora].[All]" allUniqueName="[Egzaminator].[ID Egzaminatora].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Egzaminator].[Imie I Nazwisko]" caption="Imie I Nazwisko" attribute="1" defaultMemberUniqueName="[Egzaminator].[Imie I Nazwisko].[All]" allUniqueName="[Egzaminator].[Imie I Nazwisko].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Egzaminator].[Pesel]" caption="Pesel" attribute="1" defaultMemberUniqueName="[Egzaminator].[Pesel].[All]" allUniqueName="[Egzaminator].[Pesel].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
@@ -1484,21 +1481,11 @@
     <cacheHierarchy uniqueName="[Pytanie].[ID Pytania]" caption="ID Pytania" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Pytanie].[ID Pytania].[All]" allUniqueName="[Pytanie].[ID Pytania].[All]" dimensionUniqueName="[Pytanie]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Pytanie].[Tresc]" caption="Tresc" attribute="1" defaultMemberUniqueName="[Pytanie].[Tresc].[All]" allUniqueName="[Pytanie].[Tresc].[All]" dimensionUniqueName="[Pytanie]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty]" caption="Czy Istnieja Powiazane Incydenty" attribute="1" defaultMemberUniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty].[All]" allUniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania]" caption="Czy Kandydat Odpowiedzial Na Wszystkie Pytania" attribute="1" defaultMemberUniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania].[All]" allUniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="2"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania]" caption="Czy Kandydat Odpowiedzial Na Wszystkie Pytania" attribute="1" defaultMemberUniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania].[All]" allUniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[Hierarchy]" caption="Hierarchy" defaultMemberUniqueName="[Skarga].[Hierarchy].[All]" allUniqueName="[Skarga].[Hierarchy].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[ID Skargi]" caption="ID Skargi" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Skarga].[ID Skargi].[All]" allUniqueName="[Skarga].[ID Skargi].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[Typ Egzaminu]" caption="Typ Egzaminu" attribute="1" defaultMemberUniqueName="[Skarga].[Typ Egzaminu].[All]" allUniqueName="[Skarga].[Typ Egzaminu].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Skarga].[Typ Skargi]" caption="Typ Skargi" attribute="1" defaultMemberUniqueName="[Skarga].[Typ Skargi].[All]" allUniqueName="[Skarga].[Typ Skargi].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Skarga].[Typ Skargi]" caption="Typ Skargi" attribute="1" defaultMemberUniqueName="[Skarga].[Typ Skargi].[All]" allUniqueName="[Skarga].[Typ Skargi].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Czasu]" caption="ID Czasu" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Czasu].[All]" allUniqueName="[Termin Egzaminu].[ID Czasu].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Daty]" caption="ID Daty" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Daty].[All]" allUniqueName="[Termin Egzaminu].[ID Daty].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Egzaminatora]" caption="ID Egzaminatora" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Egzaminatora].[All]" allUniqueName="[Termin Egzaminu].[ID Egzaminatora].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
@@ -1514,20 +1501,31 @@
     <cacheHierarchy uniqueName="[Measures].[Liczba egzaminów]" caption="Liczba egzaminów" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba uczestników]" caption="Łączna liczba uczestników" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba rezerwacji]" caption="Łączna liczba rezerwacji" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba skarg]" caption="Liczba skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba powiązanych incydentów]" caption="Liczba powiązanych incydentów" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba kandydatów którzy złożyli skargi]" caption="Liczba kandydatów którzy złożyli skargi" measure="1" displayFolder="" measureGroup="Zlozenie Skargi 1" count="0" oneField="1">
+    <cacheHierarchy uniqueName="[Measures].[Liczba skarg]" caption="Liczba skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" oneField="1">
       <fieldsUsage count="1">
         <fieldUsage x="0"/>
       </fieldsUsage>
     </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Liczba powiązanych incydentów]" caption="Liczba powiązanych incydentów" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Liczba kandydatów którzy złożyli skargi]" caption="Liczba kandydatów którzy złożyli skargi" measure="1" displayFolder="" measureGroup="Zlozenie Skargi 1" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba pytań]" caption="Liczba pytań" measure="1" displayFolder="" measureGroup="Odpowiedzenie Na Pytanie Podczas Egzaminu Ze Skarga" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji]" caption="Średnia liczba rezerwacji" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Średni czas oczekiwania na egzamin]" caption="Średni czas oczekiwania na egzamin" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji na kandydata]" caption="Średnia liczba rezerwacji na kandydata" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba kandydatów nieobecnych]" caption="Łączna liczba kandydatów nieobecnych" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Value]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Goal)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Status)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Trend)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Liczby Skarg Value]" caption="Zmniejszenie Liczby Skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Goal]" caption="Zmniejszenie Liczby Skarg (Goal)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Status]" caption="Zmniejszenie Liczby Skarg (Status)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Trend]" caption="Zmniejszenie Liczby Skarg (Trend)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
   </cacheHierarchies>
-  <kpis count="0"/>
+  <kpis count="2">
+    <kpi uniqueName="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" displayFolder="" measureGroup="Zarezerwowanie Terminu" parent="" value="[Measures].[Średni czas oczekiwania na egzamin]" goal="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" status="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" trend="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" weight=""/>
+    <kpi uniqueName="Zmniejszenie Liczby Skarg" caption="Zmniejszenie Liczby Skarg" displayFolder="" measureGroup="Zlozenie Skargi" parent="" value="[Measures].[Liczba skarg]" goal="[Measures].[Zmniejszenie Liczby Skarg Goal]" status="[Measures].[Zmniejszenie Liczby Skarg Status]" trend="[Measures].[Zmniejszenie Liczby Skarg Trend]" weight=""/>
+  </kpis>
   <dimensions count="9">
     <dimension name="Czas" uniqueName="[Czas]" caption="Czas"/>
     <dimension name="Data" uniqueName="[Data]" caption="Data"/>
@@ -1599,15 +1597,38 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45618.912823379629" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{AC306A8E-2BC3-446B-BB60-44BDA1DF0736}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45636.828930439813" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{6BD7594C-0175-4998-B9B3-37E5A8ED475E}">
   <cacheSource type="external" connectionId="1"/>
-  <cacheFields count="2">
-    <cacheField name="[Measures].[Liczba skarg]" caption="Liczba skarg" numFmtId="0" hierarchy="37" level="32767"/>
-    <cacheField name="[Skarga].[Czy Istnieja Powiazane Incydenty].[Czy Istnieja Powiazane Incydenty]" caption="Czy Istnieja Powiazane Incydenty" numFmtId="0" hierarchy="16" level="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+  <cacheFields count="4">
+    <cacheField name="[Measures].[Średni czas oczekiwania na egzamin]" caption="Średni czas oczekiwania na egzamin" numFmtId="0" hierarchy="42" level="32767"/>
+    <cacheField name="[Data].[Rok].[Rok]" caption="Rok" numFmtId="0" hierarchy="8" level="1">
+      <sharedItems count="1">
+        <s v="[Data].[Rok].&amp;[2021]" c="2021"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Data].[Miesiac].[Miesiac]" caption="Miesiac" numFmtId="0" hierarchy="7" level="1" mappingCount="1">
+      <sharedItems count="6">
+        <s v="[Data].[Miesiac].&amp;[Styczeń]" c="Styczeń"/>
+        <s v="[Data].[Miesiac].&amp;[Luty]" c="Luty"/>
+        <s v="[Data].[Miesiac].&amp;[Marzec]" c="Marzec"/>
+        <s v="[Data].[Miesiac].&amp;[Kwiecień]" c="Kwiecień"/>
+        <s v="[Data].[Miesiac].&amp;[Maj]" c="Maj"/>
+        <s v="[Data].[Miesiac].&amp;[Czerwiec]" c="Czerwiec"/>
+      </sharedItems>
+      <mpMap v="3"/>
+    </cacheField>
+    <cacheField name="[Data].[Miesiac].[Miesiac].[Numer Miesiaca]" caption="Numer Miesiaca" propertyName="Numer Miesiaca" numFmtId="0" hierarchy="7" level="1" memberPropertyField="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="6" count="6">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="3"/>
+        <n v="4"/>
+        <n v="5"/>
+        <n v="6"/>
+      </sharedItems>
     </cacheField>
   </cacheFields>
-  <cacheHierarchies count="45">
+  <cacheHierarchies count="53">
     <cacheHierarchy uniqueName="[Czas].[Godzina]" caption="Godzina" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Godzina].[All]" allUniqueName="[Czas].[Godzina].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[ID Czasu]" caption="ID Czasu" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Czas].[ID Czasu].[All]" allUniqueName="[Czas].[ID Czasu].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[Minuty]" caption="Minuty" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Minuty].[All]" allUniqueName="[Czas].[Minuty].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
@@ -1615,8 +1636,18 @@
     <cacheHierarchy uniqueName="[Data].[Dzien Tygodnia]" caption="Dzien Tygodnia" attribute="1" time="1" defaultMemberUniqueName="[Data].[Dzien Tygodnia].[All]" allUniqueName="[Data].[Dzien Tygodnia].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[Hierarchy]" caption="Hierarchy" time="1" defaultMemberUniqueName="[Data].[Hierarchy].[All]" allUniqueName="[Data].[Hierarchy].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[ID Daty]" caption="ID Daty" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data].[ID Daty].[All]" allUniqueName="[Data].[ID Daty].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data].[Miesiac]" caption="Miesiac" attribute="1" time="1" defaultMemberUniqueName="[Data].[Miesiac].[All]" allUniqueName="[Data].[Miesiac].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data].[Rok]" caption="Rok" attribute="1" time="1" defaultMemberUniqueName="[Data].[Rok].[All]" allUniqueName="[Data].[Rok].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data].[Miesiac]" caption="Miesiac" attribute="1" time="1" defaultMemberUniqueName="[Data].[Miesiac].[All]" allUniqueName="[Data].[Miesiac].[All]" dimensionUniqueName="[Data]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="2"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Data].[Rok]" caption="Rok" attribute="1" time="1" defaultMemberUniqueName="[Data].[Rok].[All]" allUniqueName="[Data].[Rok].[All]" dimensionUniqueName="[Data]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Egzaminator].[ID Egzaminatora]" caption="ID Egzaminatora" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Egzaminator].[ID Egzaminatora].[All]" allUniqueName="[Egzaminator].[ID Egzaminatora].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Egzaminator].[Imie I Nazwisko]" caption="Imie I Nazwisko" attribute="1" defaultMemberUniqueName="[Egzaminator].[Imie I Nazwisko].[All]" allUniqueName="[Egzaminator].[Imie I Nazwisko].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Egzaminator].[Pesel]" caption="Pesel" attribute="1" defaultMemberUniqueName="[Egzaminator].[Pesel].[All]" allUniqueName="[Egzaminator].[Pesel].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
@@ -1624,12 +1655,7 @@
     <cacheHierarchy uniqueName="[Kandydat].[PKK]" caption="PKK" attribute="1" defaultMemberUniqueName="[Kandydat].[PKK].[All]" allUniqueName="[Kandydat].[PKK].[All]" dimensionUniqueName="[Kandydat]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Pytanie].[ID Pytania]" caption="ID Pytania" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Pytanie].[ID Pytania].[All]" allUniqueName="[Pytanie].[ID Pytania].[All]" dimensionUniqueName="[Pytanie]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Pytanie].[Tresc]" caption="Tresc" attribute="1" defaultMemberUniqueName="[Pytanie].[Tresc].[All]" allUniqueName="[Pytanie].[Tresc].[All]" dimensionUniqueName="[Pytanie]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty]" caption="Czy Istnieja Powiazane Incydenty" attribute="1" defaultMemberUniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty].[All]" allUniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty]" caption="Czy Istnieja Powiazane Incydenty" attribute="1" defaultMemberUniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty].[All]" allUniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania]" caption="Czy Kandydat Odpowiedzial Na Wszystkie Pytania" attribute="1" defaultMemberUniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania].[All]" allUniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[Hierarchy]" caption="Hierarchy" defaultMemberUniqueName="[Skarga].[Hierarchy].[All]" allUniqueName="[Skarga].[Hierarchy].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[ID Skargi]" caption="ID Skargi" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Skarga].[ID Skargi].[All]" allUniqueName="[Skarga].[ID Skargi].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
@@ -1650,20 +1676,31 @@
     <cacheHierarchy uniqueName="[Measures].[Liczba egzaminów]" caption="Liczba egzaminów" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba uczestników]" caption="Łączna liczba uczestników" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba rezerwacji]" caption="Łączna liczba rezerwacji" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba skarg]" caption="Liczba skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" oneField="1">
+    <cacheHierarchy uniqueName="[Measures].[Liczba skarg]" caption="Liczba skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Liczba powiązanych incydentów]" caption="Liczba powiązanych incydentów" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Liczba kandydatów którzy złożyli skargi]" caption="Liczba kandydatów którzy złożyli skargi" measure="1" displayFolder="" measureGroup="Zlozenie Skargi 1" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Liczba pytań]" caption="Liczba pytań" measure="1" displayFolder="" measureGroup="Odpowiedzenie Na Pytanie Podczas Egzaminu Ze Skarga" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji]" caption="Średnia liczba rezerwacji" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Średni czas oczekiwania na egzamin]" caption="Średni czas oczekiwania na egzamin" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" oneField="1">
       <fieldsUsage count="1">
         <fieldUsage x="0"/>
       </fieldsUsage>
     </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Measures].[Liczba powiązanych incydentów]" caption="Liczba powiązanych incydentów" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba kandydatów którzy złożyli skargi]" caption="Liczba kandydatów którzy złożyli skargi" measure="1" displayFolder="" measureGroup="Zlozenie Skargi 1" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba pytań]" caption="Liczba pytań" measure="1" displayFolder="" measureGroup="Odpowiedzenie Na Pytanie Podczas Egzaminu Ze Skarga" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji]" caption="Średnia liczba rezerwacji" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Średni czas oczekiwania na egzamin]" caption="Średni czas oczekiwania na egzamin" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji na kandydata]" caption="Średnia liczba rezerwacji na kandydata" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba kandydatów nieobecnych]" caption="Łączna liczba kandydatów nieobecnych" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Value]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Goal)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Status)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Trend)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Liczby Skarg Value]" caption="Zmniejszenie Liczby Skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Goal]" caption="Zmniejszenie Liczby Skarg (Goal)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Status]" caption="Zmniejszenie Liczby Skarg (Status)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Trend]" caption="Zmniejszenie Liczby Skarg (Trend)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
   </cacheHierarchies>
-  <kpis count="0"/>
+  <kpis count="2">
+    <kpi uniqueName="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" displayFolder="" measureGroup="Zarezerwowanie Terminu" parent="" value="[Measures].[Średni czas oczekiwania na egzamin]" goal="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" status="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" trend="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" weight=""/>
+    <kpi uniqueName="Zmniejszenie Liczby Skarg" caption="Zmniejszenie Liczby Skarg" displayFolder="" measureGroup="Zlozenie Skargi" parent="" value="[Measures].[Liczba skarg]" goal="[Measures].[Zmniejszenie Liczby Skarg Goal]" status="[Measures].[Zmniejszenie Liczby Skarg Status]" trend="[Measures].[Zmniejszenie Liczby Skarg Trend]" weight=""/>
+  </kpis>
   <dimensions count="9">
     <dimension name="Czas" uniqueName="[Czas]" caption="Czas"/>
     <dimension name="Data" uniqueName="[Data]" caption="Data"/>
@@ -1735,29 +1772,41 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45618.912823842591" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{D8ED1B2D-A008-499B-8085-266B359926E3}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45636.828934259262" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{EAA51855-1558-401A-BF95-A8D3866F610B}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="3">
-    <cacheField name="[Measures].[Liczba skarg]" caption="Liczba skarg" numFmtId="0" hierarchy="37" level="32767"/>
-    <cacheField name="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].[Numer Sali Egzaminacyjnej]" caption="Numer Sali Egzaminacyjnej" numFmtId="0" hierarchy="26" level="1">
+    <cacheField name="[Measures].[Średnia liczba rezerwacji]" caption="Średnia liczba rezerwacji" numFmtId="0" hierarchy="41" level="32767"/>
+    <cacheField name="[Data].[Dzien Tygodnia].[Dzien Tygodnia]" caption="Dzien Tygodnia" numFmtId="0" hierarchy="4" level="1" mappingCount="1">
       <sharedItems count="5">
-        <s v="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].&amp;[162]" c="162"/>
-        <s v="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].&amp;[421]" c="421"/>
-        <s v="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].&amp;[793]" c="793"/>
-        <s v="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].&amp;[895]" c="895"/>
-        <s v="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].&amp;[979]" c="979"/>
+        <s v="[Data].[Dzien Tygodnia].&amp;[Poniedziałek]" c="Poniedziałek"/>
+        <s v="[Data].[Dzien Tygodnia].&amp;[Wtorek]" c="Wtorek"/>
+        <s v="[Data].[Dzien Tygodnia].&amp;[Środa]" c="Środa"/>
+        <s v="[Data].[Dzien Tygodnia].&amp;[Czwartek]" c="Czwartek"/>
+        <s v="[Data].[Dzien Tygodnia].&amp;[Piątek]" c="Piątek"/>
+      </sharedItems>
+      <mpMap v="2"/>
+    </cacheField>
+    <cacheField name="[Data].[Dzien Tygodnia].[Dzien Tygodnia].[Numer Dnia Tygodnia]" caption="Numer Dnia Tygodnia" propertyName="Numer Dnia Tygodnia" numFmtId="0" hierarchy="4" level="1" memberPropertyField="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="6" count="5">
+        <n v="2"/>
+        <n v="3"/>
+        <n v="4"/>
+        <n v="5"/>
+        <n v="6"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="[Skarga].[Typ Skargi].[Typ Skargi]" caption="Typ Skargi" numFmtId="0" hierarchy="21" level="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
   </cacheFields>
-  <cacheHierarchies count="45">
+  <cacheHierarchies count="53">
     <cacheHierarchy uniqueName="[Czas].[Godzina]" caption="Godzina" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Godzina].[All]" allUniqueName="[Czas].[Godzina].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[ID Czasu]" caption="ID Czasu" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Czas].[ID Czasu].[All]" allUniqueName="[Czas].[ID Czasu].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[Minuty]" caption="Minuty" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Minuty].[All]" allUniqueName="[Czas].[Minuty].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[Data]" caption="Data" attribute="1" time="1" defaultMemberUniqueName="[Data].[Data].[All]" allUniqueName="[Data].[Data].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data].[Dzien Tygodnia]" caption="Dzien Tygodnia" attribute="1" time="1" defaultMemberUniqueName="[Data].[Dzien Tygodnia].[All]" allUniqueName="[Data].[Dzien Tygodnia].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data].[Dzien Tygodnia]" caption="Dzien Tygodnia" attribute="1" time="1" defaultMemberUniqueName="[Data].[Dzien Tygodnia].[All]" allUniqueName="[Data].[Dzien Tygodnia].[All]" dimensionUniqueName="[Data]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Data].[Hierarchy]" caption="Hierarchy" time="1" defaultMemberUniqueName="[Data].[Hierarchy].[All]" allUniqueName="[Data].[Hierarchy].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[ID Daty]" caption="ID Daty" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data].[ID Daty].[All]" allUniqueName="[Data].[ID Daty].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[Miesiac]" caption="Miesiac" attribute="1" time="1" defaultMemberUniqueName="[Data].[Miesiac].[All]" allUniqueName="[Data].[Miesiac].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
@@ -1774,22 +1823,12 @@
     <cacheHierarchy uniqueName="[Skarga].[Hierarchy]" caption="Hierarchy" defaultMemberUniqueName="[Skarga].[Hierarchy].[All]" allUniqueName="[Skarga].[Hierarchy].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[ID Skargi]" caption="ID Skargi" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Skarga].[ID Skargi].[All]" allUniqueName="[Skarga].[ID Skargi].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[Typ Egzaminu]" caption="Typ Egzaminu" attribute="1" defaultMemberUniqueName="[Skarga].[Typ Egzaminu].[All]" allUniqueName="[Skarga].[Typ Egzaminu].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Skarga].[Typ Skargi]" caption="Typ Skargi" attribute="1" defaultMemberUniqueName="[Skarga].[Typ Skargi].[All]" allUniqueName="[Skarga].[Typ Skargi].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="2"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Skarga].[Typ Skargi]" caption="Typ Skargi" attribute="1" defaultMemberUniqueName="[Skarga].[Typ Skargi].[All]" allUniqueName="[Skarga].[Typ Skargi].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Czasu]" caption="ID Czasu" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Czasu].[All]" allUniqueName="[Termin Egzaminu].[ID Czasu].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Daty]" caption="ID Daty" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Daty].[All]" allUniqueName="[Termin Egzaminu].[ID Daty].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Egzaminatora]" caption="ID Egzaminatora" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Egzaminatora].[All]" allUniqueName="[Termin Egzaminu].[ID Egzaminatora].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Terminu Egzaminu]" caption="ID Terminu Egzaminu" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Terminu Egzaminu].[All]" allUniqueName="[Termin Egzaminu].[ID Terminu Egzaminu].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Termin Egzaminu].[Numer Sali Egzaminacyjnej]" caption="Numer Sali Egzaminacyjnej" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].[All]" allUniqueName="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Termin Egzaminu].[Numer Sali Egzaminacyjnej]" caption="Numer Sali Egzaminacyjnej" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].[All]" allUniqueName="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Zajetosc Terminu Egzaminu].[ID Zajetosci Terminu Egzaminu]" caption="ID Zajetosci Terminu Egzaminu" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Zajetosc Terminu Egzaminu].[ID Zajetosci Terminu Egzaminu].[All]" allUniqueName="[Zajetosc Terminu Egzaminu].[ID Zajetosci Terminu Egzaminu].[All]" dimensionUniqueName="[Zajetosc Terminu Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Zajetosc Terminu Egzaminu].[Zajetosc Terminu]" caption="Zajetosc Terminu" attribute="1" defaultMemberUniqueName="[Zajetosc Terminu Egzaminu].[Zajetosc Terminu].[All]" allUniqueName="[Zajetosc Terminu Egzaminu].[Zajetosc Terminu].[All]" dimensionUniqueName="[Zajetosc Terminu Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba rezerwacji na termin]" caption="Liczba rezerwacji na termin" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
@@ -1800,20 +1839,31 @@
     <cacheHierarchy uniqueName="[Measures].[Liczba egzaminów]" caption="Liczba egzaminów" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba uczestników]" caption="Łączna liczba uczestników" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba rezerwacji]" caption="Łączna liczba rezerwacji" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba skarg]" caption="Liczba skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" oneField="1">
+    <cacheHierarchy uniqueName="[Measures].[Liczba skarg]" caption="Liczba skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Liczba powiązanych incydentów]" caption="Liczba powiązanych incydentów" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Liczba kandydatów którzy złożyli skargi]" caption="Liczba kandydatów którzy złożyli skargi" measure="1" displayFolder="" measureGroup="Zlozenie Skargi 1" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Liczba pytań]" caption="Liczba pytań" measure="1" displayFolder="" measureGroup="Odpowiedzenie Na Pytanie Podczas Egzaminu Ze Skarga" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji]" caption="Średnia liczba rezerwacji" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" oneField="1">
       <fieldsUsage count="1">
         <fieldUsage x="0"/>
       </fieldsUsage>
     </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Measures].[Liczba powiązanych incydentów]" caption="Liczba powiązanych incydentów" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba kandydatów którzy złożyli skargi]" caption="Liczba kandydatów którzy złożyli skargi" measure="1" displayFolder="" measureGroup="Zlozenie Skargi 1" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba pytań]" caption="Liczba pytań" measure="1" displayFolder="" measureGroup="Odpowiedzenie Na Pytanie Podczas Egzaminu Ze Skarga" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji]" caption="Średnia liczba rezerwacji" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Średni czas oczekiwania na egzamin]" caption="Średni czas oczekiwania na egzamin" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji na kandydata]" caption="Średnia liczba rezerwacji na kandydata" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba kandydatów nieobecnych]" caption="Łączna liczba kandydatów nieobecnych" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Value]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Goal)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Status)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Trend)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Liczby Skarg Value]" caption="Zmniejszenie Liczby Skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Goal]" caption="Zmniejszenie Liczby Skarg (Goal)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Status]" caption="Zmniejszenie Liczby Skarg (Status)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Trend]" caption="Zmniejszenie Liczby Skarg (Trend)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
   </cacheHierarchies>
-  <kpis count="0"/>
+  <kpis count="2">
+    <kpi uniqueName="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" displayFolder="" measureGroup="Zarezerwowanie Terminu" parent="" value="[Measures].[Średni czas oczekiwania na egzamin]" goal="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" status="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" trend="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" weight=""/>
+    <kpi uniqueName="Zmniejszenie Liczby Skarg" caption="Zmniejszenie Liczby Skarg" displayFolder="" measureGroup="Zlozenie Skargi" parent="" value="[Measures].[Liczba skarg]" goal="[Measures].[Zmniejszenie Liczby Skarg Goal]" status="[Measures].[Zmniejszenie Liczby Skarg Status]" trend="[Measures].[Zmniejszenie Liczby Skarg Trend]" weight=""/>
+  </kpis>
   <dimensions count="9">
     <dimension name="Czas" uniqueName="[Czas]" caption="Czas"/>
     <dimension name="Data" uniqueName="[Data]" caption="Data"/>
@@ -1885,38 +1935,63 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45618.912824421299" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{965E1953-E265-4900-A23F-F48C3B3F6EDB}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45636.828937500002" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{6B514316-8103-42FA-B301-BBAE9F6A1E04}">
   <cacheSource type="external" connectionId="1"/>
-  <cacheFields count="4">
-    <cacheField name="[Measures].[Łączna liczba kandydatów nieobecnych]" caption="Łączna liczba kandydatów nieobecnych" numFmtId="0" hierarchy="44" level="32767"/>
-    <cacheField name="[Data].[Rok].[Rok]" caption="Rok" numFmtId="0" hierarchy="8" level="1">
-      <sharedItems count="1">
-        <s v="[Data].[Rok].&amp;[2021]" c="2021"/>
-      </sharedItems>
+  <cacheFields count="3">
+    <cacheField name="[Measures].[Liczba pytań]" caption="Liczba pytań" numFmtId="0" hierarchy="40" level="32767"/>
+    <cacheField name="[Skarga].[Typ Skargi].[Typ Skargi]" caption="Typ Skargi" numFmtId="0" hierarchy="21" level="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
     </cacheField>
-    <cacheField name="[Data].[Miesiac].[Miesiac]" caption="Miesiac" numFmtId="0" hierarchy="7" level="1" mappingCount="1">
-      <sharedItems count="6">
-        <s v="[Data].[Miesiac].&amp;[Styczeń]" c="Styczeń"/>
-        <s v="[Data].[Miesiac].&amp;[Luty]" c="Luty"/>
-        <s v="[Data].[Miesiac].&amp;[Marzec]" c="Marzec"/>
-        <s v="[Data].[Miesiac].&amp;[Kwiecień]" c="Kwiecień"/>
-        <s v="[Data].[Miesiac].&amp;[Maj]" c="Maj"/>
-        <s v="[Data].[Miesiac].&amp;[Czerwiec]" c="Czerwiec"/>
-      </sharedItems>
-      <mpMap v="3"/>
-    </cacheField>
-    <cacheField name="[Data].[Miesiac].[Miesiac].[Numer Miesiaca]" caption="Numer Miesiaca" propertyName="Numer Miesiaca" numFmtId="0" hierarchy="7" level="1" memberPropertyField="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="6" count="6">
-        <n v="1"/>
-        <n v="2"/>
-        <n v="3"/>
-        <n v="4"/>
-        <n v="5"/>
-        <n v="6"/>
+    <cacheField name="[Pytanie].[Tresc].[Tresc]" caption="Tresc" numFmtId="0" hierarchy="15" level="1">
+      <sharedItems count="44">
+        <s v="[Pytanie].[Tresc].&amp;[Co należy zrobić, gdy widzimy pojazd uprzywilejowany?]" c="Co należy zrobić, gdy widzimy pojazd uprzywilejowany?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co należy zrobić, gdy widzimy znak 'Droga jednokierunkowa'?]" c="Co należy zrobić, gdy widzimy znak 'Droga jednokierunkowa'?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co należy zrobić, gdy widzimy znak 'Przejście dla pieszych'?]" c="Co należy zrobić, gdy widzimy znak 'Przejście dla pieszych'?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co należy zrobić, gdy widzimy znak 'Stop'?]" c="Co należy zrobić, gdy widzimy znak 'Stop'?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co należy zrobić, gdy widzimy znak 'Ustąp pierwszeństwa'?]" c="Co należy zrobić, gdy widzimy znak 'Ustąp pierwszeństwa'?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co należy zrobić, gdy widzimy znak 'Zakaz wjazdu rowerów'?]" c="Co należy zrobić, gdy widzimy znak 'Zakaz wjazdu rowerów'?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co należy zrobić, gdy widzimy znak 'Zakaz wjazdu'?]" c="Co należy zrobić, gdy widzimy znak 'Zakaz wjazdu'?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co należy zrobić, gdy zbliżamy się do przejścia dla pieszych?]" c="Co należy zrobić, gdy zbliżamy się do przejścia dla pieszych?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co oznacza czerwone światło na sygnalizatorze?]" c="Co oznacza czerwone światło na sygnalizatorze?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co oznacza zielone światło na sygnalizatorze?]" c="Co oznacza zielone światło na sygnalizatorze?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Droga dla pieszych'?]" c="Co oznacza znak 'Droga dla pieszych'?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Koniec autostrady'?]" c="Co oznacza znak 'Koniec autostrady'?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Obowiązkowy kierunek jazdy'?]" c="Co oznacza znak 'Obowiązkowy kierunek jazdy'?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak ograniczenie prędkości?]" c="Co oznacza znak ograniczenie prędkości?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Przejazd kolejowy z zaporami'?]" c="Co oznacza znak 'Przejazd kolejowy z zaporami'?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Uwaga, dzieci'?]" c="Co oznacza znak 'Uwaga, dzieci'?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Zakaz skrętu w lewo'?]" c="Co oznacza znak 'Zakaz skrętu w lewo'?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Zakaz wjazdu motocykli'?]" c="Co oznacza znak 'Zakaz wjazdu motocykli'?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Zakaz wjazdu przyczep'?]" c="Co oznacza znak 'Zakaz wjazdu przyczep'?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Zakaz wjazdu samochodów ciężarowych'?]" c="Co oznacza znak 'Zakaz wjazdu samochodów ciężarowych'?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak zakaz wjazdu?]" c="Co oznacza znak zakaz wjazdu?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Zakaz wyprzedzania samochodów ciężarowych'?]" c="Co oznacza znak 'Zakaz wyprzedzania samochodów ciężarowych'?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Zakaz wyprzedzania'?]" c="Co oznacza znak 'Zakaz wyprzedzania'?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Zakaz zatrzymywania się'?]" c="Co oznacza znak 'Zakaz zatrzymywania się'?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Znak ostrzegawczy' z symbolem skrzyżowania?]" c="Co oznacza znak 'Znak ostrzegawczy' z symbolem skrzyżowania?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Czy można korzystać z telefonu podczas prowadzenia pojazdu?]" c="Czy można korzystać z telefonu podczas prowadzenia pojazdu?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Czy można parkować na chodniku?]" c="Czy można parkować na chodniku?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Czy można prowadzić pojazd bez ubezpieczenia?]" c="Czy można prowadzić pojazd bez ubezpieczenia?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Czy można wyprzedzać na przejściu dla pieszych?]" c="Czy można wyprzedzać na przejściu dla pieszych?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Jakie jest dopuszczalne ciśnienie w oponach?]" c="Jakie jest dopuszczalne ciśnienie w oponach?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Jakie jest minimalne ciśnienie w oponach?]" c="Jakie jest minimalne ciśnienie w oponach?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Jakie jest ograniczenie prędkości na drodze ekspresowej?]" c="Jakie jest ograniczenie prędkości na drodze ekspresowej?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Jakie jest ograniczenie prędkości na drodze krajowej?]" c="Jakie jest ograniczenie prędkości na drodze krajowej?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Jakie jest ograniczenie prędkości w strefie zamieszkania?]" c="Jakie jest ograniczenie prędkości w strefie zamieszkania?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Jakie jest pierwszeństwo na rondzie?]" c="Jakie jest pierwszeństwo na rondzie?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Jakie są objawy aquaplaningu?]" c="Jakie są objawy aquaplaningu?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Jakie są zasady parkowania na chodniku?]" c="Jakie są zasady parkowania na chodniku?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Jakie są zasady używania świateł drogowych poza terenem zabudowanym?]" c="Jakie są zasady używania świateł drogowych poza terenem zabudowanym?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Jakie są zasady używania świateł drogowych?]" c="Jakie są zasady używania świateł drogowych?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Jakie są zasady używania świateł mijania w dzień?]" c="Jakie są zasady używania świateł mijania w dzień?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Jakie są zasady używania świateł mijania w nocy?]" c="Jakie są zasady używania świateł mijania w nocy?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Jakie są zasady używania świateł przeciwmgielnych?]" c="Jakie są zasady używania świateł przeciwmgielnych?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Kiedy można używać klaksonu?]" c="Kiedy można używać klaksonu?"/>
+        <s v="[Pytanie].[Tresc].&amp;[Kiedy należy używać świateł przeciwmgielnych?]" c="Kiedy należy używać świateł przeciwmgielnych?"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
-  <cacheHierarchies count="45">
+  <cacheHierarchies count="53">
     <cacheHierarchy uniqueName="[Czas].[Godzina]" caption="Godzina" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Godzina].[All]" allUniqueName="[Czas].[Godzina].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[ID Czasu]" caption="ID Czasu" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Czas].[ID Czasu].[All]" allUniqueName="[Czas].[ID Czasu].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[Minuty]" caption="Minuty" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Minuty].[All]" allUniqueName="[Czas].[Minuty].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
@@ -1924,31 +1999,31 @@
     <cacheHierarchy uniqueName="[Data].[Dzien Tygodnia]" caption="Dzien Tygodnia" attribute="1" time="1" defaultMemberUniqueName="[Data].[Dzien Tygodnia].[All]" allUniqueName="[Data].[Dzien Tygodnia].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[Hierarchy]" caption="Hierarchy" time="1" defaultMemberUniqueName="[Data].[Hierarchy].[All]" allUniqueName="[Data].[Hierarchy].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[ID Daty]" caption="ID Daty" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data].[ID Daty].[All]" allUniqueName="[Data].[ID Daty].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data].[Miesiac]" caption="Miesiac" attribute="1" time="1" defaultMemberUniqueName="[Data].[Miesiac].[All]" allUniqueName="[Data].[Miesiac].[All]" dimensionUniqueName="[Data]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="2"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Data].[Rok]" caption="Rok" attribute="1" time="1" defaultMemberUniqueName="[Data].[Rok].[All]" allUniqueName="[Data].[Rok].[All]" dimensionUniqueName="[Data]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Data].[Miesiac]" caption="Miesiac" attribute="1" time="1" defaultMemberUniqueName="[Data].[Miesiac].[All]" allUniqueName="[Data].[Miesiac].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data].[Rok]" caption="Rok" attribute="1" time="1" defaultMemberUniqueName="[Data].[Rok].[All]" allUniqueName="[Data].[Rok].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Egzaminator].[ID Egzaminatora]" caption="ID Egzaminatora" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Egzaminator].[ID Egzaminatora].[All]" allUniqueName="[Egzaminator].[ID Egzaminatora].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Egzaminator].[Imie I Nazwisko]" caption="Imie I Nazwisko" attribute="1" defaultMemberUniqueName="[Egzaminator].[Imie I Nazwisko].[All]" allUniqueName="[Egzaminator].[Imie I Nazwisko].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Egzaminator].[Pesel]" caption="Pesel" attribute="1" defaultMemberUniqueName="[Egzaminator].[Pesel].[All]" allUniqueName="[Egzaminator].[Pesel].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Kandydat].[ID Kandydata]" caption="ID Kandydata" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Kandydat].[ID Kandydata].[All]" allUniqueName="[Kandydat].[ID Kandydata].[All]" dimensionUniqueName="[Kandydat]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Kandydat].[PKK]" caption="PKK" attribute="1" defaultMemberUniqueName="[Kandydat].[PKK].[All]" allUniqueName="[Kandydat].[PKK].[All]" dimensionUniqueName="[Kandydat]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Pytanie].[ID Pytania]" caption="ID Pytania" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Pytanie].[ID Pytania].[All]" allUniqueName="[Pytanie].[ID Pytania].[All]" dimensionUniqueName="[Pytanie]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Pytanie].[Tresc]" caption="Tresc" attribute="1" defaultMemberUniqueName="[Pytanie].[Tresc].[All]" allUniqueName="[Pytanie].[Tresc].[All]" dimensionUniqueName="[Pytanie]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Pytanie].[Tresc]" caption="Tresc" attribute="1" defaultMemberUniqueName="[Pytanie].[Tresc].[All]" allUniqueName="[Pytanie].[Tresc].[All]" dimensionUniqueName="[Pytanie]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="2"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty]" caption="Czy Istnieja Powiazane Incydenty" attribute="1" defaultMemberUniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty].[All]" allUniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania]" caption="Czy Kandydat Odpowiedzial Na Wszystkie Pytania" attribute="1" defaultMemberUniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania].[All]" allUniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[Hierarchy]" caption="Hierarchy" defaultMemberUniqueName="[Skarga].[Hierarchy].[All]" allUniqueName="[Skarga].[Hierarchy].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[ID Skargi]" caption="ID Skargi" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Skarga].[ID Skargi].[All]" allUniqueName="[Skarga].[ID Skargi].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[Typ Egzaminu]" caption="Typ Egzaminu" attribute="1" defaultMemberUniqueName="[Skarga].[Typ Egzaminu].[All]" allUniqueName="[Skarga].[Typ Egzaminu].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Skarga].[Typ Skargi]" caption="Typ Skargi" attribute="1" defaultMemberUniqueName="[Skarga].[Typ Skargi].[All]" allUniqueName="[Skarga].[Typ Skargi].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Skarga].[Typ Skargi]" caption="Typ Skargi" attribute="1" defaultMemberUniqueName="[Skarga].[Typ Skargi].[All]" allUniqueName="[Skarga].[Typ Skargi].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Czasu]" caption="ID Czasu" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Czasu].[All]" allUniqueName="[Termin Egzaminu].[ID Czasu].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Daty]" caption="ID Daty" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Daty].[All]" allUniqueName="[Termin Egzaminu].[ID Daty].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Egzaminatora]" caption="ID Egzaminatora" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Egzaminatora].[All]" allUniqueName="[Termin Egzaminu].[ID Egzaminatora].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
@@ -1967,17 +2042,28 @@
     <cacheHierarchy uniqueName="[Measures].[Liczba skarg]" caption="Liczba skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba powiązanych incydentów]" caption="Liczba powiązanych incydentów" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba kandydatów którzy złożyli skargi]" caption="Liczba kandydatów którzy złożyli skargi" measure="1" displayFolder="" measureGroup="Zlozenie Skargi 1" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba pytań]" caption="Liczba pytań" measure="1" displayFolder="" measureGroup="Odpowiedzenie Na Pytanie Podczas Egzaminu Ze Skarga" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji]" caption="Średnia liczba rezerwacji" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Średni czas oczekiwania na egzamin]" caption="Średni czas oczekiwania na egzamin" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji na kandydata]" caption="Średnia liczba rezerwacji na kandydata" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Łączna liczba kandydatów nieobecnych]" caption="Łączna liczba kandydatów nieobecnych" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0" oneField="1">
+    <cacheHierarchy uniqueName="[Measures].[Liczba pytań]" caption="Liczba pytań" measure="1" displayFolder="" measureGroup="Odpowiedzenie Na Pytanie Podczas Egzaminu Ze Skarga" count="0" oneField="1">
       <fieldsUsage count="1">
         <fieldUsage x="0"/>
       </fieldsUsage>
     </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji]" caption="Średnia liczba rezerwacji" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Średni czas oczekiwania na egzamin]" caption="Średni czas oczekiwania na egzamin" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji na kandydata]" caption="Średnia liczba rezerwacji na kandydata" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Łączna liczba kandydatów nieobecnych]" caption="Łączna liczba kandydatów nieobecnych" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Value]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Goal)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Status)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Trend)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Liczby Skarg Value]" caption="Zmniejszenie Liczby Skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Goal]" caption="Zmniejszenie Liczby Skarg (Goal)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Status]" caption="Zmniejszenie Liczby Skarg (Status)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Trend]" caption="Zmniejszenie Liczby Skarg (Trend)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
   </cacheHierarchies>
-  <kpis count="0"/>
+  <kpis count="2">
+    <kpi uniqueName="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" displayFolder="" measureGroup="Zarezerwowanie Terminu" parent="" value="[Measures].[Średni czas oczekiwania na egzamin]" goal="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" status="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" trend="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" weight=""/>
+    <kpi uniqueName="Zmniejszenie Liczby Skarg" caption="Zmniejszenie Liczby Skarg" displayFolder="" measureGroup="Zlozenie Skargi" parent="" value="[Measures].[Liczba skarg]" goal="[Measures].[Zmniejszenie Liczby Skarg Goal]" status="[Measures].[Zmniejszenie Liczby Skarg Status]" trend="[Measures].[Zmniejszenie Liczby Skarg Trend]" weight=""/>
+  </kpis>
   <dimensions count="9">
     <dimension name="Czas" uniqueName="[Czas]" caption="Czas"/>
     <dimension name="Data" uniqueName="[Data]" caption="Data"/>
@@ -2049,7 +2135,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45618.912824999999" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{3D05820F-88AE-46FE-9E60-268CB7FD8052}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45636.828939699073" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{3D05820F-88AE-46FE-9E60-268CB7FD8052}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="4">
     <cacheField name="[Measures].[Średnia liczba rezerwacji na kandydata]" caption="Średnia liczba rezerwacji na kandydata" numFmtId="0" hierarchy="43" level="32767"/>
@@ -2080,7 +2166,7 @@
       </sharedItems>
     </cacheField>
   </cacheFields>
-  <cacheHierarchies count="45">
+  <cacheHierarchies count="53">
     <cacheHierarchy uniqueName="[Czas].[Godzina]" caption="Godzina" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Godzina].[All]" allUniqueName="[Czas].[Godzina].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[ID Czasu]" caption="ID Czasu" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Czas].[ID Czasu].[All]" allUniqueName="[Czas].[ID Czasu].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[Minuty]" caption="Minuty" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Minuty].[All]" allUniqueName="[Czas].[Minuty].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
@@ -2140,8 +2226,19 @@
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba kandydatów nieobecnych]" caption="Łączna liczba kandydatów nieobecnych" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Value]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Goal)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Status)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Trend)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Liczby Skarg Value]" caption="Zmniejszenie Liczby Skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Goal]" caption="Zmniejszenie Liczby Skarg (Goal)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Status]" caption="Zmniejszenie Liczby Skarg (Status)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Trend]" caption="Zmniejszenie Liczby Skarg (Trend)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
   </cacheHierarchies>
-  <kpis count="0"/>
+  <kpis count="2">
+    <kpi uniqueName="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" displayFolder="" measureGroup="Zarezerwowanie Terminu" parent="" value="[Measures].[Średni czas oczekiwania na egzamin]" goal="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" status="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" trend="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" weight=""/>
+    <kpi uniqueName="Zmniejszenie Liczby Skarg" caption="Zmniejszenie Liczby Skarg" displayFolder="" measureGroup="Zlozenie Skargi" parent="" value="[Measures].[Liczba skarg]" goal="[Measures].[Zmniejszenie Liczby Skarg Goal]" status="[Measures].[Zmniejszenie Liczby Skarg Status]" trend="[Measures].[Zmniejszenie Liczby Skarg Trend]" weight=""/>
+  </kpis>
   <dimensions count="9">
     <dimension name="Czas" uniqueName="[Czas]" caption="Czas"/>
     <dimension name="Data" uniqueName="[Data]" caption="Data"/>
@@ -2213,77 +2310,38 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45618.912826273146" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{6B514316-8103-42FA-B301-BBAE9F6A1E04}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45636.828945138892" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{965E1953-E265-4900-A23F-F48C3B3F6EDB}">
   <cacheSource type="external" connectionId="1"/>
-  <cacheFields count="3">
-    <cacheField name="[Measures].[Liczba pytań]" caption="Liczba pytań" numFmtId="0" hierarchy="40" level="32767"/>
-    <cacheField name="[Skarga].[Typ Skargi].[Typ Skargi]" caption="Typ Skargi" numFmtId="0" hierarchy="21" level="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+  <cacheFields count="4">
+    <cacheField name="[Measures].[Łączna liczba kandydatów nieobecnych]" caption="Łączna liczba kandydatów nieobecnych" numFmtId="0" hierarchy="44" level="32767"/>
+    <cacheField name="[Data].[Rok].[Rok]" caption="Rok" numFmtId="0" hierarchy="8" level="1">
+      <sharedItems count="1">
+        <s v="[Data].[Rok].&amp;[2021]" c="2021"/>
+      </sharedItems>
     </cacheField>
-    <cacheField name="[Pytanie].[Tresc].[Tresc]" caption="Tresc" numFmtId="0" hierarchy="15" level="1">
-      <sharedItems count="58">
-        <s v="[Pytanie].[Tresc].&amp;[Co należy zrobić w przypadku awarii na autostradzie?]" c="Co należy zrobić w przypadku awarii na autostradzie?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co należy zrobić, gdy widzimy pojazd uprzywilejowany?]" c="Co należy zrobić, gdy widzimy pojazd uprzywilejowany?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co należy zrobić, gdy widzimy znak 'Droga jednokierunkowa'?]" c="Co należy zrobić, gdy widzimy znak 'Droga jednokierunkowa'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co należy zrobić, gdy widzimy znak 'Przejście dla pieszych'?]" c="Co należy zrobić, gdy widzimy znak 'Przejście dla pieszych'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co należy zrobić, gdy widzimy znak 'Stop'?]" c="Co należy zrobić, gdy widzimy znak 'Stop'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co należy zrobić, gdy widzimy znak 'Ustąp pierwszeństwa'?]" c="Co należy zrobić, gdy widzimy znak 'Ustąp pierwszeństwa'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co należy zrobić, gdy widzimy znak 'Zakaz parkowania'?]" c="Co należy zrobić, gdy widzimy znak 'Zakaz parkowania'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co należy zrobić, gdy widzimy znak 'Zakaz wjazdu rowerów'?]" c="Co należy zrobić, gdy widzimy znak 'Zakaz wjazdu rowerów'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co należy zrobić, gdy widzimy znak 'Zakaz wjazdu'?]" c="Co należy zrobić, gdy widzimy znak 'Zakaz wjazdu'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co należy zrobić, gdy zbliżamy się do przejścia dla pieszych?]" c="Co należy zrobić, gdy zbliżamy się do przejścia dla pieszych?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co oznacza czerwone światło na sygnalizatorze?]" c="Co oznacza czerwone światło na sygnalizatorze?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co oznacza zielone światło na sygnalizatorze?]" c="Co oznacza zielone światło na sygnalizatorze?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Droga dla pieszych'?]" c="Co oznacza znak 'Droga dla pieszych'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Droga dla rowerów'?]" c="Co oznacza znak 'Droga dla rowerów'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Droga z pierwszeństwem'?]" c="Co oznacza znak 'Droga z pierwszeństwem'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Koniec autostrady'?]" c="Co oznacza znak 'Koniec autostrady'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Koniec ograniczenia prędkości'?]" c="Co oznacza znak 'Koniec ograniczenia prędkości'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Obowiązkowy kierunek jazdy'?]" c="Co oznacza znak 'Obowiązkowy kierunek jazdy'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak ograniczenie prędkości?]" c="Co oznacza znak ograniczenie prędkości?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Przejazd kolejowy z zaporami'?]" c="Co oznacza znak 'Przejazd kolejowy z zaporami'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Uwaga, dzieci'?]" c="Co oznacza znak 'Uwaga, dzieci'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Zakaz skrętu w lewo'?]" c="Co oznacza znak 'Zakaz skrętu w lewo'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Zakaz wjazdu motocykli'?]" c="Co oznacza znak 'Zakaz wjazdu motocykli'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Zakaz wjazdu przyczep'?]" c="Co oznacza znak 'Zakaz wjazdu przyczep'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Zakaz wjazdu rowerów'?]" c="Co oznacza znak 'Zakaz wjazdu rowerów'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Zakaz wjazdu samochodów ciężarowych'?]" c="Co oznacza znak 'Zakaz wjazdu samochodów ciężarowych'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak zakaz wjazdu?]" c="Co oznacza znak zakaz wjazdu?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Zakaz wyprzedzania samochodów ciężarowych'?]" c="Co oznacza znak 'Zakaz wyprzedzania samochodów ciężarowych'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Zakaz wyprzedzania'?]" c="Co oznacza znak 'Zakaz wyprzedzania'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Zakaz zatrzymywania się'?]" c="Co oznacza znak 'Zakaz zatrzymywania się'?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Co oznacza znak 'Znak ostrzegawczy' z symbolem skrzyżowania?]" c="Co oznacza znak 'Znak ostrzegawczy' z symbolem skrzyżowania?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Czy można korzystać z telefonu podczas prowadzenia pojazdu?]" c="Czy można korzystać z telefonu podczas prowadzenia pojazdu?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Czy można parkować na chodniku?]" c="Czy można parkować na chodniku?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Czy można prowadzić pojazd bez ubezpieczenia?]" c="Czy można prowadzić pojazd bez ubezpieczenia?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Czy można wyprzedzać na przejściu dla pieszych?]" c="Czy można wyprzedzać na przejściu dla pieszych?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Czy można wyprzedzać na skrzyżowaniu?]" c="Czy można wyprzedzać na skrzyżowaniu?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Czy można wyprzedzać pojazd na przejściu dla pieszych?]" c="Czy można wyprzedzać pojazd na przejściu dla pieszych?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Jakie jest dopuszczalne ciśnienie w oponach?]" c="Jakie jest dopuszczalne ciśnienie w oponach?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Jakie jest maksymalne dopuszczalne stężenie alkoholu we krwi kierowcy w Polsce?]" c="Jakie jest maksymalne dopuszczalne stężenie alkoholu we krwi kierowcy w Polsce?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Jakie jest minimalne ciśnienie w oponach?]" c="Jakie jest minimalne ciśnienie w oponach?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Jakie jest minimalne ogumienie dozwolone na samochodzie osobowym?]" c="Jakie jest minimalne ogumienie dozwolone na samochodzie osobowym?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Jakie jest ograniczenie prędkości na autostradzie?]" c="Jakie jest ograniczenie prędkości na autostradzie?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Jakie jest ograniczenie prędkości na drodze ekspresowej?]" c="Jakie jest ograniczenie prędkości na drodze ekspresowej?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Jakie jest ograniczenie prędkości na drodze krajowej?]" c="Jakie jest ograniczenie prędkości na drodze krajowej?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Jakie jest ograniczenie prędkości w strefie zamieszkania?]" c="Jakie jest ograniczenie prędkości w strefie zamieszkania?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Jakie jest ograniczenie prędkości w terenie zabudowanym?]" c="Jakie jest ograniczenie prędkości w terenie zabudowanym?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Jakie jest pierwszeństwo na rondzie?]" c="Jakie jest pierwszeństwo na rondzie?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Jakie są objawy aquaplaningu?]" c="Jakie są objawy aquaplaningu?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Jakie są zasady parkowania na chodniku?]" c="Jakie są zasady parkowania na chodniku?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Jakie są zasady używania świateł drogowych poza terenem zabudowanym?]" c="Jakie są zasady używania świateł drogowych poza terenem zabudowanym?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Jakie są zasady używania świateł drogowych?]" c="Jakie są zasady używania świateł drogowych?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Jakie są zasady używania świateł mijania w dzień?]" c="Jakie są zasady używania świateł mijania w dzień?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Jakie są zasady używania świateł mijania w nocy?]" c="Jakie są zasady używania świateł mijania w nocy?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Jakie są zasady używania świateł mijania?]" c="Jakie są zasady używania świateł mijania?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Jakie są zasady używania świateł przeciwmgielnych?]" c="Jakie są zasady używania świateł przeciwmgielnych?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Kiedy można używać klaksonu?]" c="Kiedy można używać klaksonu?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Kiedy należy używać pasów bezpieczeństwa?]" c="Kiedy należy używać pasów bezpieczeństwa?"/>
-        <s v="[Pytanie].[Tresc].&amp;[Kiedy należy używać świateł przeciwmgielnych?]" c="Kiedy należy używać świateł przeciwmgielnych?"/>
+    <cacheField name="[Data].[Miesiac].[Miesiac]" caption="Miesiac" numFmtId="0" hierarchy="7" level="1" mappingCount="1">
+      <sharedItems count="6">
+        <s v="[Data].[Miesiac].&amp;[Styczeń]" c="Styczeń"/>
+        <s v="[Data].[Miesiac].&amp;[Luty]" c="Luty"/>
+        <s v="[Data].[Miesiac].&amp;[Marzec]" c="Marzec"/>
+        <s v="[Data].[Miesiac].&amp;[Kwiecień]" c="Kwiecień"/>
+        <s v="[Data].[Miesiac].&amp;[Maj]" c="Maj"/>
+        <s v="[Data].[Miesiac].&amp;[Czerwiec]" c="Czerwiec"/>
+      </sharedItems>
+      <mpMap v="3"/>
+    </cacheField>
+    <cacheField name="[Data].[Miesiac].[Miesiac].[Numer Miesiaca]" caption="Numer Miesiaca" propertyName="Numer Miesiaca" numFmtId="0" hierarchy="7" level="1" memberPropertyField="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="6" count="6">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="3"/>
+        <n v="4"/>
+        <n v="5"/>
+        <n v="6"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
-  <cacheHierarchies count="45">
+  <cacheHierarchies count="53">
     <cacheHierarchy uniqueName="[Czas].[Godzina]" caption="Godzina" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Godzina].[All]" allUniqueName="[Czas].[Godzina].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[ID Czasu]" caption="ID Czasu" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Czas].[ID Czasu].[All]" allUniqueName="[Czas].[ID Czasu].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[Minuty]" caption="Minuty" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Minuty].[All]" allUniqueName="[Czas].[Minuty].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
@@ -2291,31 +2349,31 @@
     <cacheHierarchy uniqueName="[Data].[Dzien Tygodnia]" caption="Dzien Tygodnia" attribute="1" time="1" defaultMemberUniqueName="[Data].[Dzien Tygodnia].[All]" allUniqueName="[Data].[Dzien Tygodnia].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[Hierarchy]" caption="Hierarchy" time="1" defaultMemberUniqueName="[Data].[Hierarchy].[All]" allUniqueName="[Data].[Hierarchy].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[ID Daty]" caption="ID Daty" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data].[ID Daty].[All]" allUniqueName="[Data].[ID Daty].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data].[Miesiac]" caption="Miesiac" attribute="1" time="1" defaultMemberUniqueName="[Data].[Miesiac].[All]" allUniqueName="[Data].[Miesiac].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data].[Rok]" caption="Rok" attribute="1" time="1" defaultMemberUniqueName="[Data].[Rok].[All]" allUniqueName="[Data].[Rok].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data].[Miesiac]" caption="Miesiac" attribute="1" time="1" defaultMemberUniqueName="[Data].[Miesiac].[All]" allUniqueName="[Data].[Miesiac].[All]" dimensionUniqueName="[Data]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="2"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Data].[Rok]" caption="Rok" attribute="1" time="1" defaultMemberUniqueName="[Data].[Rok].[All]" allUniqueName="[Data].[Rok].[All]" dimensionUniqueName="[Data]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Egzaminator].[ID Egzaminatora]" caption="ID Egzaminatora" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Egzaminator].[ID Egzaminatora].[All]" allUniqueName="[Egzaminator].[ID Egzaminatora].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Egzaminator].[Imie I Nazwisko]" caption="Imie I Nazwisko" attribute="1" defaultMemberUniqueName="[Egzaminator].[Imie I Nazwisko].[All]" allUniqueName="[Egzaminator].[Imie I Nazwisko].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Egzaminator].[Pesel]" caption="Pesel" attribute="1" defaultMemberUniqueName="[Egzaminator].[Pesel].[All]" allUniqueName="[Egzaminator].[Pesel].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Kandydat].[ID Kandydata]" caption="ID Kandydata" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Kandydat].[ID Kandydata].[All]" allUniqueName="[Kandydat].[ID Kandydata].[All]" dimensionUniqueName="[Kandydat]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Kandydat].[PKK]" caption="PKK" attribute="1" defaultMemberUniqueName="[Kandydat].[PKK].[All]" allUniqueName="[Kandydat].[PKK].[All]" dimensionUniqueName="[Kandydat]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Pytanie].[ID Pytania]" caption="ID Pytania" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Pytanie].[ID Pytania].[All]" allUniqueName="[Pytanie].[ID Pytania].[All]" dimensionUniqueName="[Pytanie]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Pytanie].[Tresc]" caption="Tresc" attribute="1" defaultMemberUniqueName="[Pytanie].[Tresc].[All]" allUniqueName="[Pytanie].[Tresc].[All]" dimensionUniqueName="[Pytanie]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="2"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Pytanie].[Tresc]" caption="Tresc" attribute="1" defaultMemberUniqueName="[Pytanie].[Tresc].[All]" allUniqueName="[Pytanie].[Tresc].[All]" dimensionUniqueName="[Pytanie]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty]" caption="Czy Istnieja Powiazane Incydenty" attribute="1" defaultMemberUniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty].[All]" allUniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania]" caption="Czy Kandydat Odpowiedzial Na Wszystkie Pytania" attribute="1" defaultMemberUniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania].[All]" allUniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[Hierarchy]" caption="Hierarchy" defaultMemberUniqueName="[Skarga].[Hierarchy].[All]" allUniqueName="[Skarga].[Hierarchy].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[ID Skargi]" caption="ID Skargi" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Skarga].[ID Skargi].[All]" allUniqueName="[Skarga].[ID Skargi].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[Typ Egzaminu]" caption="Typ Egzaminu" attribute="1" defaultMemberUniqueName="[Skarga].[Typ Egzaminu].[All]" allUniqueName="[Skarga].[Typ Egzaminu].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Skarga].[Typ Skargi]" caption="Typ Skargi" attribute="1" defaultMemberUniqueName="[Skarga].[Typ Skargi].[All]" allUniqueName="[Skarga].[Typ Skargi].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Skarga].[Typ Skargi]" caption="Typ Skargi" attribute="1" defaultMemberUniqueName="[Skarga].[Typ Skargi].[All]" allUniqueName="[Skarga].[Typ Skargi].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Czasu]" caption="ID Czasu" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Czasu].[All]" allUniqueName="[Termin Egzaminu].[ID Czasu].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Daty]" caption="ID Daty" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Daty].[All]" allUniqueName="[Termin Egzaminu].[ID Daty].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Egzaminatora]" caption="ID Egzaminatora" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Egzaminatora].[All]" allUniqueName="[Termin Egzaminu].[ID Egzaminatora].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
@@ -2334,17 +2392,28 @@
     <cacheHierarchy uniqueName="[Measures].[Liczba skarg]" caption="Liczba skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba powiązanych incydentów]" caption="Liczba powiązanych incydentów" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba kandydatów którzy złożyli skargi]" caption="Liczba kandydatów którzy złożyli skargi" measure="1" displayFolder="" measureGroup="Zlozenie Skargi 1" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba pytań]" caption="Liczba pytań" measure="1" displayFolder="" measureGroup="Odpowiedzenie Na Pytanie Podczas Egzaminu Ze Skarga" count="0" oneField="1">
+    <cacheHierarchy uniqueName="[Measures].[Liczba pytań]" caption="Liczba pytań" measure="1" displayFolder="" measureGroup="Odpowiedzenie Na Pytanie Podczas Egzaminu Ze Skarga" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji]" caption="Średnia liczba rezerwacji" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Średni czas oczekiwania na egzamin]" caption="Średni czas oczekiwania na egzamin" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji na kandydata]" caption="Średnia liczba rezerwacji na kandydata" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Łączna liczba kandydatów nieobecnych]" caption="Łączna liczba kandydatów nieobecnych" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0" oneField="1">
       <fieldsUsage count="1">
         <fieldUsage x="0"/>
       </fieldsUsage>
     </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji]" caption="Średnia liczba rezerwacji" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Średni czas oczekiwania na egzamin]" caption="Średni czas oczekiwania na egzamin" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji na kandydata]" caption="Średnia liczba rezerwacji na kandydata" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Łączna liczba kandydatów nieobecnych]" caption="Łączna liczba kandydatów nieobecnych" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Value]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Goal)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Status)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Trend)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Liczby Skarg Value]" caption="Zmniejszenie Liczby Skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Goal]" caption="Zmniejszenie Liczby Skarg (Goal)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Status]" caption="Zmniejszenie Liczby Skarg (Status)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Trend]" caption="Zmniejszenie Liczby Skarg (Trend)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
   </cacheHierarchies>
-  <kpis count="0"/>
+  <kpis count="2">
+    <kpi uniqueName="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" displayFolder="" measureGroup="Zarezerwowanie Terminu" parent="" value="[Measures].[Średni czas oczekiwania na egzamin]" goal="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" status="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" trend="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" weight=""/>
+    <kpi uniqueName="Zmniejszenie Liczby Skarg" caption="Zmniejszenie Liczby Skarg" displayFolder="" measureGroup="Zlozenie Skargi" parent="" value="[Measures].[Liczba skarg]" goal="[Measures].[Zmniejszenie Liczby Skarg Goal]" status="[Measures].[Zmniejszenie Liczby Skarg Status]" trend="[Measures].[Zmniejszenie Liczby Skarg Trend]" weight=""/>
+  </kpis>
   <dimensions count="9">
     <dimension name="Czas" uniqueName="[Czas]" caption="Czas"/>
     <dimension name="Data" uniqueName="[Data]" caption="Data"/>
@@ -2416,41 +2485,29 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45618.912826967593" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{EAA51855-1558-401A-BF95-A8D3866F610B}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45636.828948148148" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{D8ED1B2D-A008-499B-8085-266B359926E3}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="3">
-    <cacheField name="[Measures].[Średnia liczba rezerwacji]" caption="Średnia liczba rezerwacji" numFmtId="0" hierarchy="41" level="32767"/>
-    <cacheField name="[Data].[Dzien Tygodnia].[Dzien Tygodnia]" caption="Dzien Tygodnia" numFmtId="0" hierarchy="4" level="1" mappingCount="1">
+    <cacheField name="[Measures].[Liczba skarg]" caption="Liczba skarg" numFmtId="0" hierarchy="37" level="32767"/>
+    <cacheField name="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].[Numer Sali Egzaminacyjnej]" caption="Numer Sali Egzaminacyjnej" numFmtId="0" hierarchy="26" level="1">
       <sharedItems count="5">
-        <s v="[Data].[Dzien Tygodnia].&amp;[Poniedziałek]" c="Poniedziałek"/>
-        <s v="[Data].[Dzien Tygodnia].&amp;[Wtorek]" c="Wtorek"/>
-        <s v="[Data].[Dzien Tygodnia].&amp;[Środa]" c="Środa"/>
-        <s v="[Data].[Dzien Tygodnia].&amp;[Czwartek]" c="Czwartek"/>
-        <s v="[Data].[Dzien Tygodnia].&amp;[Piątek]" c="Piątek"/>
-      </sharedItems>
-      <mpMap v="2"/>
-    </cacheField>
-    <cacheField name="[Data].[Dzien Tygodnia].[Dzien Tygodnia].[Numer Dnia Tygodnia]" caption="Numer Dnia Tygodnia" propertyName="Numer Dnia Tygodnia" numFmtId="0" hierarchy="4" level="1" memberPropertyField="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="6" count="5">
-        <n v="2"/>
-        <n v="3"/>
-        <n v="4"/>
-        <n v="5"/>
-        <n v="6"/>
+        <s v="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].&amp;[162]" c="162"/>
+        <s v="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].&amp;[421]" c="421"/>
+        <s v="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].&amp;[793]" c="793"/>
+        <s v="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].&amp;[895]" c="895"/>
+        <s v="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].&amp;[979]" c="979"/>
       </sharedItems>
     </cacheField>
+    <cacheField name="[Skarga].[Typ Skargi].[Typ Skargi]" caption="Typ Skargi" numFmtId="0" hierarchy="21" level="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
   </cacheFields>
-  <cacheHierarchies count="45">
+  <cacheHierarchies count="53">
     <cacheHierarchy uniqueName="[Czas].[Godzina]" caption="Godzina" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Godzina].[All]" allUniqueName="[Czas].[Godzina].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[ID Czasu]" caption="ID Czasu" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Czas].[ID Czasu].[All]" allUniqueName="[Czas].[ID Czasu].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[Minuty]" caption="Minuty" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Minuty].[All]" allUniqueName="[Czas].[Minuty].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[Data]" caption="Data" attribute="1" time="1" defaultMemberUniqueName="[Data].[Data].[All]" allUniqueName="[Data].[Data].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data].[Dzien Tygodnia]" caption="Dzien Tygodnia" attribute="1" time="1" defaultMemberUniqueName="[Data].[Dzien Tygodnia].[All]" allUniqueName="[Data].[Dzien Tygodnia].[All]" dimensionUniqueName="[Data]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Data].[Dzien Tygodnia]" caption="Dzien Tygodnia" attribute="1" time="1" defaultMemberUniqueName="[Data].[Dzien Tygodnia].[All]" allUniqueName="[Data].[Dzien Tygodnia].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[Hierarchy]" caption="Hierarchy" time="1" defaultMemberUniqueName="[Data].[Hierarchy].[All]" allUniqueName="[Data].[Hierarchy].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[ID Daty]" caption="ID Daty" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data].[ID Daty].[All]" allUniqueName="[Data].[ID Daty].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[Miesiac]" caption="Miesiac" attribute="1" time="1" defaultMemberUniqueName="[Data].[Miesiac].[All]" allUniqueName="[Data].[Miesiac].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
@@ -2467,12 +2524,22 @@
     <cacheHierarchy uniqueName="[Skarga].[Hierarchy]" caption="Hierarchy" defaultMemberUniqueName="[Skarga].[Hierarchy].[All]" allUniqueName="[Skarga].[Hierarchy].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[ID Skargi]" caption="ID Skargi" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Skarga].[ID Skargi].[All]" allUniqueName="[Skarga].[ID Skargi].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[Typ Egzaminu]" caption="Typ Egzaminu" attribute="1" defaultMemberUniqueName="[Skarga].[Typ Egzaminu].[All]" allUniqueName="[Skarga].[Typ Egzaminu].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Skarga].[Typ Skargi]" caption="Typ Skargi" attribute="1" defaultMemberUniqueName="[Skarga].[Typ Skargi].[All]" allUniqueName="[Skarga].[Typ Skargi].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Skarga].[Typ Skargi]" caption="Typ Skargi" attribute="1" defaultMemberUniqueName="[Skarga].[Typ Skargi].[All]" allUniqueName="[Skarga].[Typ Skargi].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="2"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Czasu]" caption="ID Czasu" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Czasu].[All]" allUniqueName="[Termin Egzaminu].[ID Czasu].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Daty]" caption="ID Daty" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Daty].[All]" allUniqueName="[Termin Egzaminu].[ID Daty].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Egzaminatora]" caption="ID Egzaminatora" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Egzaminatora].[All]" allUniqueName="[Termin Egzaminu].[ID Egzaminatora].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Termin Egzaminu].[ID Terminu Egzaminu]" caption="ID Terminu Egzaminu" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Termin Egzaminu].[ID Terminu Egzaminu].[All]" allUniqueName="[Termin Egzaminu].[ID Terminu Egzaminu].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Termin Egzaminu].[Numer Sali Egzaminacyjnej]" caption="Numer Sali Egzaminacyjnej" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].[All]" allUniqueName="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Termin Egzaminu].[Numer Sali Egzaminacyjnej]" caption="Numer Sali Egzaminacyjnej" attribute="1" defaultMemberUniqueName="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].[All]" allUniqueName="[Termin Egzaminu].[Numer Sali Egzaminacyjnej].[All]" dimensionUniqueName="[Termin Egzaminu]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Zajetosc Terminu Egzaminu].[ID Zajetosci Terminu Egzaminu]" caption="ID Zajetosci Terminu Egzaminu" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Zajetosc Terminu Egzaminu].[ID Zajetosci Terminu Egzaminu].[All]" allUniqueName="[Zajetosc Terminu Egzaminu].[ID Zajetosci Terminu Egzaminu].[All]" dimensionUniqueName="[Zajetosc Terminu Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Zajetosc Terminu Egzaminu].[Zajetosc Terminu]" caption="Zajetosc Terminu" attribute="1" defaultMemberUniqueName="[Zajetosc Terminu Egzaminu].[Zajetosc Terminu].[All]" allUniqueName="[Zajetosc Terminu Egzaminu].[Zajetosc Terminu].[All]" dimensionUniqueName="[Zajetosc Terminu Egzaminu]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba rezerwacji na termin]" caption="Liczba rezerwacji na termin" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
@@ -2483,20 +2550,31 @@
     <cacheHierarchy uniqueName="[Measures].[Liczba egzaminów]" caption="Liczba egzaminów" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba uczestników]" caption="Łączna liczba uczestników" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba rezerwacji]" caption="Łączna liczba rezerwacji" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba skarg]" caption="Liczba skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba powiązanych incydentów]" caption="Liczba powiązanych incydentów" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba kandydatów którzy złożyli skargi]" caption="Liczba kandydatów którzy złożyli skargi" measure="1" displayFolder="" measureGroup="Zlozenie Skargi 1" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba pytań]" caption="Liczba pytań" measure="1" displayFolder="" measureGroup="Odpowiedzenie Na Pytanie Podczas Egzaminu Ze Skarga" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji]" caption="Średnia liczba rezerwacji" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" oneField="1">
+    <cacheHierarchy uniqueName="[Measures].[Liczba skarg]" caption="Liczba skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" oneField="1">
       <fieldsUsage count="1">
         <fieldUsage x="0"/>
       </fieldsUsage>
     </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Liczba powiązanych incydentów]" caption="Liczba powiązanych incydentów" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Liczba kandydatów którzy złożyli skargi]" caption="Liczba kandydatów którzy złożyli skargi" measure="1" displayFolder="" measureGroup="Zlozenie Skargi 1" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Liczba pytań]" caption="Liczba pytań" measure="1" displayFolder="" measureGroup="Odpowiedzenie Na Pytanie Podczas Egzaminu Ze Skarga" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji]" caption="Średnia liczba rezerwacji" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Średni czas oczekiwania na egzamin]" caption="Średni czas oczekiwania na egzamin" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji na kandydata]" caption="Średnia liczba rezerwacji na kandydata" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba kandydatów nieobecnych]" caption="Łączna liczba kandydatów nieobecnych" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Value]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Goal)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Status)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Trend)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Liczby Skarg Value]" caption="Zmniejszenie Liczby Skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Goal]" caption="Zmniejszenie Liczby Skarg (Goal)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Status]" caption="Zmniejszenie Liczby Skarg (Status)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Trend]" caption="Zmniejszenie Liczby Skarg (Trend)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
   </cacheHierarchies>
-  <kpis count="0"/>
+  <kpis count="2">
+    <kpi uniqueName="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" displayFolder="" measureGroup="Zarezerwowanie Terminu" parent="" value="[Measures].[Średni czas oczekiwania na egzamin]" goal="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" status="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" trend="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" weight=""/>
+    <kpi uniqueName="Zmniejszenie Liczby Skarg" caption="Zmniejszenie Liczby Skarg" displayFolder="" measureGroup="Zlozenie Skargi" parent="" value="[Measures].[Liczba skarg]" goal="[Measures].[Zmniejszenie Liczby Skarg Goal]" status="[Measures].[Zmniejszenie Liczby Skarg Status]" trend="[Measures].[Zmniejszenie Liczby Skarg Trend]" weight=""/>
+  </kpis>
   <dimensions count="9">
     <dimension name="Czas" uniqueName="[Czas]" caption="Czas"/>
     <dimension name="Data" uniqueName="[Data]" caption="Data"/>
@@ -2568,38 +2646,15 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45618.912827546294" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{6BD7594C-0175-4998-B9B3-37E5A8ED475E}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="KanarekLife" refreshedDate="45636.82895127315" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{AC306A8E-2BC3-446B-BB60-44BDA1DF0736}">
   <cacheSource type="external" connectionId="1"/>
-  <cacheFields count="4">
-    <cacheField name="[Measures].[Średni czas oczekiwania na egzamin]" caption="Średni czas oczekiwania na egzamin" numFmtId="0" hierarchy="42" level="32767"/>
-    <cacheField name="[Data].[Rok].[Rok]" caption="Rok" numFmtId="0" hierarchy="8" level="1">
-      <sharedItems count="1">
-        <s v="[Data].[Rok].&amp;[2021]" c="2021"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Data].[Miesiac].[Miesiac]" caption="Miesiac" numFmtId="0" hierarchy="7" level="1" mappingCount="1">
-      <sharedItems count="6">
-        <s v="[Data].[Miesiac].&amp;[Styczeń]" c="Styczeń"/>
-        <s v="[Data].[Miesiac].&amp;[Luty]" c="Luty"/>
-        <s v="[Data].[Miesiac].&amp;[Marzec]" c="Marzec"/>
-        <s v="[Data].[Miesiac].&amp;[Kwiecień]" c="Kwiecień"/>
-        <s v="[Data].[Miesiac].&amp;[Maj]" c="Maj"/>
-        <s v="[Data].[Miesiac].&amp;[Czerwiec]" c="Czerwiec"/>
-      </sharedItems>
-      <mpMap v="3"/>
-    </cacheField>
-    <cacheField name="[Data].[Miesiac].[Miesiac].[Numer Miesiaca]" caption="Numer Miesiaca" propertyName="Numer Miesiaca" numFmtId="0" hierarchy="7" level="1" memberPropertyField="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="6" count="6">
-        <n v="1"/>
-        <n v="2"/>
-        <n v="3"/>
-        <n v="4"/>
-        <n v="5"/>
-        <n v="6"/>
-      </sharedItems>
+  <cacheFields count="2">
+    <cacheField name="[Measures].[Liczba skarg]" caption="Liczba skarg" numFmtId="0" hierarchy="37" level="32767"/>
+    <cacheField name="[Skarga].[Czy Istnieja Powiazane Incydenty].[Czy Istnieja Powiazane Incydenty]" caption="Czy Istnieja Powiazane Incydenty" numFmtId="0" hierarchy="16" level="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
     </cacheField>
   </cacheFields>
-  <cacheHierarchies count="45">
+  <cacheHierarchies count="53">
     <cacheHierarchy uniqueName="[Czas].[Godzina]" caption="Godzina" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Godzina].[All]" allUniqueName="[Czas].[Godzina].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[ID Czasu]" caption="ID Czasu" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Czas].[ID Czasu].[All]" allUniqueName="[Czas].[ID Czasu].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Czas].[Minuty]" caption="Minuty" attribute="1" time="1" defaultMemberUniqueName="[Czas].[Minuty].[All]" allUniqueName="[Czas].[Minuty].[All]" dimensionUniqueName="[Czas]" displayFolder="" count="0" unbalanced="0"/>
@@ -2607,18 +2662,8 @@
     <cacheHierarchy uniqueName="[Data].[Dzien Tygodnia]" caption="Dzien Tygodnia" attribute="1" time="1" defaultMemberUniqueName="[Data].[Dzien Tygodnia].[All]" allUniqueName="[Data].[Dzien Tygodnia].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[Hierarchy]" caption="Hierarchy" time="1" defaultMemberUniqueName="[Data].[Hierarchy].[All]" allUniqueName="[Data].[Hierarchy].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Data].[ID Daty]" caption="ID Daty" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Data].[ID Daty].[All]" allUniqueName="[Data].[ID Daty].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" memberValueDatatype="3" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Data].[Miesiac]" caption="Miesiac" attribute="1" time="1" defaultMemberUniqueName="[Data].[Miesiac].[All]" allUniqueName="[Data].[Miesiac].[All]" dimensionUniqueName="[Data]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="2"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Data].[Rok]" caption="Rok" attribute="1" time="1" defaultMemberUniqueName="[Data].[Rok].[All]" allUniqueName="[Data].[Rok].[All]" dimensionUniqueName="[Data]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Data].[Miesiac]" caption="Miesiac" attribute="1" time="1" defaultMemberUniqueName="[Data].[Miesiac].[All]" allUniqueName="[Data].[Miesiac].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Data].[Rok]" caption="Rok" attribute="1" time="1" defaultMemberUniqueName="[Data].[Rok].[All]" allUniqueName="[Data].[Rok].[All]" dimensionUniqueName="[Data]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Egzaminator].[ID Egzaminatora]" caption="ID Egzaminatora" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Egzaminator].[ID Egzaminatora].[All]" allUniqueName="[Egzaminator].[ID Egzaminatora].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Egzaminator].[Imie I Nazwisko]" caption="Imie I Nazwisko" attribute="1" defaultMemberUniqueName="[Egzaminator].[Imie I Nazwisko].[All]" allUniqueName="[Egzaminator].[Imie I Nazwisko].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Egzaminator].[Pesel]" caption="Pesel" attribute="1" defaultMemberUniqueName="[Egzaminator].[Pesel].[All]" allUniqueName="[Egzaminator].[Pesel].[All]" dimensionUniqueName="[Egzaminator]" displayFolder="" count="0" unbalanced="0"/>
@@ -2626,7 +2671,12 @@
     <cacheHierarchy uniqueName="[Kandydat].[PKK]" caption="PKK" attribute="1" defaultMemberUniqueName="[Kandydat].[PKK].[All]" allUniqueName="[Kandydat].[PKK].[All]" dimensionUniqueName="[Kandydat]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Pytanie].[ID Pytania]" caption="ID Pytania" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Pytanie].[ID Pytania].[All]" allUniqueName="[Pytanie].[ID Pytania].[All]" dimensionUniqueName="[Pytanie]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Pytanie].[Tresc]" caption="Tresc" attribute="1" defaultMemberUniqueName="[Pytanie].[Tresc].[All]" allUniqueName="[Pytanie].[Tresc].[All]" dimensionUniqueName="[Pytanie]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty]" caption="Czy Istnieja Powiazane Incydenty" attribute="1" defaultMemberUniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty].[All]" allUniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty]" caption="Czy Istnieja Powiazane Incydenty" attribute="1" defaultMemberUniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty].[All]" allUniqueName="[Skarga].[Czy Istnieja Powiazane Incydenty].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania]" caption="Czy Kandydat Odpowiedzial Na Wszystkie Pytania" attribute="1" defaultMemberUniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania].[All]" allUniqueName="[Skarga].[Czy Kandydat Odpowiedzial Na Wszystkie Pytania].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[Hierarchy]" caption="Hierarchy" defaultMemberUniqueName="[Skarga].[Hierarchy].[All]" allUniqueName="[Skarga].[Hierarchy].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Skarga].[ID Skargi]" caption="ID Skargi" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Skarga].[ID Skargi].[All]" allUniqueName="[Skarga].[ID Skargi].[All]" dimensionUniqueName="[Skarga]" displayFolder="" count="0" unbalanced="0"/>
@@ -2647,20 +2697,31 @@
     <cacheHierarchy uniqueName="[Measures].[Liczba egzaminów]" caption="Liczba egzaminów" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba uczestników]" caption="Łączna liczba uczestników" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba rezerwacji]" caption="Łączna liczba rezerwacji" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Liczba skarg]" caption="Liczba skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Liczba skarg]" caption="Liczba skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[Liczba powiązanych incydentów]" caption="Liczba powiązanych incydentów" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba kandydatów którzy złożyli skargi]" caption="Liczba kandydatów którzy złożyli skargi" measure="1" displayFolder="" measureGroup="Zlozenie Skargi 1" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Liczba pytań]" caption="Liczba pytań" measure="1" displayFolder="" measureGroup="Odpowiedzenie Na Pytanie Podczas Egzaminu Ze Skarga" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji]" caption="Średnia liczba rezerwacji" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Średni czas oczekiwania na egzamin]" caption="Średni czas oczekiwania na egzamin" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" oneField="1">
-      <fieldsUsage count="1">
-        <fieldUsage x="0"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Średni czas oczekiwania na egzamin]" caption="Średni czas oczekiwania na egzamin" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Średnia liczba rezerwacji na kandydata]" caption="Średnia liczba rezerwacji na kandydata" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Łączna liczba kandydatów nieobecnych]" caption="Łączna liczba kandydatów nieobecnych" measure="1" displayFolder="" measureGroup="Odbycie Sie Egzaminu" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Value]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Goal)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Status)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu (Trend)" measure="1" displayFolder="" measureGroup="Zarezerwowanie Terminu" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[___Zmniejszenie Liczby Skarg Value]" caption="Zmniejszenie Liczby Skarg" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Goal]" caption="Zmniejszenie Liczby Skarg (Goal)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Status]" caption="Zmniejszenie Liczby Skarg (Status)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Zmniejszenie Liczby Skarg Trend]" caption="Zmniejszenie Liczby Skarg (Trend)" measure="1" displayFolder="" measureGroup="Zlozenie Skargi" count="0" hidden="1"/>
   </cacheHierarchies>
-  <kpis count="0"/>
+  <kpis count="2">
+    <kpi uniqueName="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" caption="Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu" displayFolder="" measureGroup="Zarezerwowanie Terminu" parent="" value="[Measures].[Średni czas oczekiwania na egzamin]" goal="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Goal]" status="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Status]" trend="[Measures].[Zmniejszenie Średniego Czasu Oczekiwania na Termin Egzaminu Trend]" weight=""/>
+    <kpi uniqueName="Zmniejszenie Liczby Skarg" caption="Zmniejszenie Liczby Skarg" displayFolder="" measureGroup="Zlozenie Skargi" parent="" value="[Measures].[Liczba skarg]" goal="[Measures].[Zmniejszenie Liczby Skarg Goal]" status="[Measures].[Zmniejszenie Liczby Skarg Status]" trend="[Measures].[Zmniejszenie Liczby Skarg Trend]" weight=""/>
+  </kpis>
   <dimensions count="9">
     <dimension name="Czas" uniqueName="[Czas]" caption="Czas"/>
     <dimension name="Data" uniqueName="[Data]" caption="Data"/>
@@ -2732,7 +2793,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{55103A3D-AB2F-410A-BFC7-F37972FB508E}" name="Tabela przestawna2" cacheId="106" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{55103A3D-AB2F-410A-BFC7-F37972FB508E}" name="Tabela przestawna2" cacheId="250" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -2789,7 +2850,7 @@
   <dataFields count="1">
     <dataField fld="0" baseField="0" baseItem="0"/>
   </dataFields>
-  <pivotHierarchies count="45">
+  <pivotHierarchies count="55">
     <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
@@ -2839,6 +2900,16 @@
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
   </pivotHierarchies>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <rowHierarchiesUsage count="2">
@@ -2857,7 +2928,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6AC1A645-D905-4686-885A-18B06F13B08F}" name="Tabela przestawna11" cacheId="85" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6AC1A645-D905-4686-885A-18B06F13B08F}" name="Tabela przestawna11" cacheId="268" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A3:A4" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -2875,52 +2946,62 @@
   <dataFields count="1">
     <dataField fld="0" baseField="0" baseItem="0"/>
   </dataFields>
-  <pivotHierarchies count="45">
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+  <pivotHierarchies count="55">
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
   </pivotHierarchies>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -2935,7 +3016,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ABDFE37C-A315-4E97-9E22-9A3C4E804529}" name="Tabela przestawna12" cacheId="82" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{ABDFE37C-A315-4E97-9E22-9A3C4E804529}" name="Tabela przestawna12" cacheId="271" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A4:A5" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -2955,7 +3036,7 @@
   <dataFields count="1">
     <dataField fld="0" baseField="0" baseItem="0"/>
   </dataFields>
-  <pivotHierarchies count="45">
+  <pivotHierarchies count="55">
     <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
@@ -3006,6 +3087,16 @@
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
   </pivotHierarchies>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -3020,8 +3111,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{03CC55A2-2A79-4877-B00F-7D11D7F354D6}" name="Tabela przestawna3" cacheId="109" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
-  <location ref="A1:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{03CC55A2-2A79-4877-B00F-7D11D7F354D6}" name="Tabela przestawna3" cacheId="247" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+  <location ref="A1:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -3030,12 +3121,10 @@
       </items>
     </pivotField>
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
-      <items count="5">
+      <items count="3">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
       </items>
     </pivotField>
     <pivotField subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" showPropTip="1"/>
@@ -3044,7 +3133,7 @@
     <field x="1"/>
     <field x="2"/>
   </rowFields>
-  <rowItems count="7">
+  <rowItems count="5">
     <i>
       <x/>
     </i>
@@ -3056,12 +3145,6 @@
     </i>
     <i r="1">
       <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="4"/>
     </i>
     <i t="grand">
       <x/>
@@ -3073,7 +3156,7 @@
   <dataFields count="1">
     <dataField fld="0" baseField="0" baseItem="0"/>
   </dataFields>
-  <pivotHierarchies count="45">
+  <pivotHierarchies count="55">
     <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
@@ -3123,6 +3206,16 @@
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
   </pivotHierarchies>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <rowHierarchiesUsage count="2">
@@ -3141,7 +3234,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7352233A-20C6-42ED-B9F7-99BFBA8C95C0}" name="Tabela przestawna4" cacheId="103" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7352233A-20C6-42ED-B9F7-99BFBA8C95C0}" name="Tabela przestawna4" cacheId="253" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -3185,7 +3278,7 @@
   <dataFields count="1">
     <dataField fld="0" baseField="0" baseItem="0"/>
   </dataFields>
-  <pivotHierarchies count="45">
+  <pivotHierarchies count="55">
     <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
@@ -3235,6 +3328,16 @@
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
   </pivotHierarchies>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <rowHierarchiesUsage count="1">
@@ -3252,7 +3355,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{12484503-3E65-4FEE-9C7F-6299D4F5B102}" name="Tabela przestawna5" cacheId="91" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{12484503-3E65-4FEE-9C7F-6299D4F5B102}" name="Tabela przestawna5" cacheId="262" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -3309,7 +3412,7 @@
   <dataFields count="1">
     <dataField fld="0" baseField="0" baseItem="0"/>
   </dataFields>
-  <pivotHierarchies count="45">
+  <pivotHierarchies count="55">
     <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
@@ -3359,6 +3462,16 @@
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
   </pivotHierarchies>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <rowHierarchiesUsage count="2">
@@ -3377,7 +3490,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8090F95E-C009-476D-A29B-114E888E0BAC}" name="Tabela przestawna6" cacheId="94" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8090F95E-C009-476D-A29B-114E888E0BAC}" name="Tabela przestawna6" cacheId="259" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -3434,7 +3547,7 @@
   <dataFields count="1">
     <dataField fld="0" baseField="0" baseItem="0"/>
   </dataFields>
-  <pivotHierarchies count="45">
+  <pivotHierarchies count="55">
     <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
@@ -3484,6 +3597,16 @@
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
   </pivotHierarchies>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <rowHierarchiesUsage count="2">
@@ -3502,7 +3625,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4B207FE6-CB9C-485B-BA76-CAAE9F938CE3}" name="Tabela przestawna7" cacheId="79" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4B207FE6-CB9C-485B-BA76-CAAE9F938CE3}" name="Tabela przestawna7" cacheId="274" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -3560,7 +3683,7 @@
   <dataFields count="1">
     <dataField fld="0" baseField="0" baseItem="0"/>
   </dataFields>
-  <pivotHierarchies count="45">
+  <pivotHierarchies count="55">
     <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
@@ -3610,6 +3733,16 @@
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
   </pivotHierarchies>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <rowHierarchiesUsage count="1">
@@ -3627,7 +3760,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5E2D5957-C94E-44CA-8CC3-C05216CAD892}" name="Tabela przestawna8" cacheId="88" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5E2D5957-C94E-44CA-8CC3-C05216CAD892}" name="Tabela przestawna8" cacheId="265" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -3674,52 +3807,62 @@
   <dataFields count="1">
     <dataField fld="0" baseField="0" baseItem="0"/>
   </dataFields>
-  <pivotHierarchies count="45">
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+  <pivotHierarchies count="55">
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
   </pivotHierarchies>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <rowHierarchiesUsage count="1">
@@ -3737,13 +3880,13 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{92A79929-FF76-4EDC-A690-BFBA82F967F4}" name="Tabela przestawna9" cacheId="100" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
-  <location ref="A4:B63" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{92A79929-FF76-4EDC-A690-BFBA82F967F4}" name="Tabela przestawna9" cacheId="256" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+  <location ref="A4:B49" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisPage" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1"/>
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
-      <items count="58">
+      <items count="44">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -3788,27 +3931,13 @@
         <item x="41"/>
         <item x="42"/>
         <item x="43"/>
-        <item x="44"/>
-        <item x="45"/>
-        <item x="46"/>
-        <item x="47"/>
-        <item x="48"/>
-        <item x="49"/>
-        <item x="50"/>
-        <item x="51"/>
-        <item x="52"/>
-        <item x="53"/>
-        <item x="54"/>
-        <item x="55"/>
-        <item x="56"/>
-        <item x="57"/>
       </items>
     </pivotField>
   </pivotFields>
   <rowFields count="1">
     <field x="2"/>
   </rowFields>
-  <rowItems count="59">
+  <rowItems count="45">
     <i>
       <x/>
     </i>
@@ -3940,48 +4069,6 @@
     </i>
     <i>
       <x v="43"/>
-    </i>
-    <i>
-      <x v="44"/>
-    </i>
-    <i>
-      <x v="45"/>
-    </i>
-    <i>
-      <x v="46"/>
-    </i>
-    <i>
-      <x v="47"/>
-    </i>
-    <i>
-      <x v="48"/>
-    </i>
-    <i>
-      <x v="49"/>
-    </i>
-    <i>
-      <x v="50"/>
-    </i>
-    <i>
-      <x v="51"/>
-    </i>
-    <i>
-      <x v="52"/>
-    </i>
-    <i>
-      <x v="53"/>
-    </i>
-    <i>
-      <x v="54"/>
-    </i>
-    <i>
-      <x v="55"/>
-    </i>
-    <i>
-      <x v="56"/>
-    </i>
-    <i>
-      <x v="57"/>
     </i>
     <i t="grand">
       <x/>
@@ -3996,52 +4083,62 @@
   <dataFields count="1">
     <dataField fld="0" baseField="0" baseItem="0"/>
   </dataFields>
-  <pivotHierarchies count="45">
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+  <pivotHierarchies count="55">
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
   </pivotHierarchies>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <rowHierarchiesUsage count="1">
@@ -4059,7 +4156,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{24AB3054-8C01-40A0-93F3-A039E8162503}" name="Tabela przestawna10" cacheId="112" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{24AB3054-8C01-40A0-93F3-A039E8162503}" name="Tabela przestawna10" cacheId="244" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -4122,52 +4219,62 @@
   <dataFields count="1">
     <dataField fld="0" baseField="0" baseItem="0"/>
   </dataFields>
-  <pivotHierarchies count="45">
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+  <pivotHierarchies count="55">
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragOff="0"/>
   </pivotHierarchies>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <rowHierarchiesUsage count="1">
@@ -4539,7 +4646,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="4">
-        <v>19.974800245851259</v>
+        <v>19.939530906425606</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -4552,7 +4659,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B8" s="4">
         <v>21.618733772718194</v>
@@ -4563,7 +4670,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="4">
-        <v>20.117084987551308</v>
+        <v>20.110453914056549</v>
       </c>
     </row>
   </sheetData>
@@ -4600,7 +4707,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
-        <v>46</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -4645,7 +4752,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4655,7 +4762,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D880E4-2621-4FC4-8DEC-27E0368A0A53}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
@@ -4683,50 +4790,34 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" s="4">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="4">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" s="4">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
+      <c r="A6" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="B6" s="4">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="4">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="4">
-        <v>107</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -4761,7 +4852,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="4">
-        <v>12.354080221300139</v>
+        <v>12.365145228215768</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -4769,7 +4860,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="4">
-        <v>12.12912087912088</v>
+        <v>12.145604395604396</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -4777,7 +4868,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="4">
-        <v>12.394444444444444</v>
+        <v>12.408333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -4785,7 +4876,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="4">
-        <v>12.379694019471488</v>
+        <v>12.392211404728791</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -4793,7 +4884,7 @@
         <v>30</v>
       </c>
       <c r="B6" s="4">
-        <v>12.107671601615074</v>
+        <v>12.123822341857336</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -4801,7 +4892,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="4">
-        <v>12.271676300578035</v>
+        <v>12.285714285714286</v>
       </c>
     </row>
   </sheetData>
@@ -4843,7 +4934,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="4">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -4851,7 +4942,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="4">
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -4859,7 +4950,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="4">
-        <v>1800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -4867,7 +4958,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="4">
-        <v>24905</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -4880,7 +4971,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B8" s="4">
         <v>25035</v>
@@ -4891,7 +4982,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="4">
-        <v>53875</v>
+        <v>27105</v>
       </c>
     </row>
   </sheetData>
@@ -4957,7 +5048,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="4">
-        <v>12.671339563862928</v>
+        <v>12.750778816199377</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -4970,7 +5061,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B8" s="4">
         <v>9.1535648994515544</v>
@@ -4981,7 +5072,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="4">
-        <v>12.271676300578035</v>
+        <v>12.285714285714286</v>
       </c>
     </row>
   </sheetData>
@@ -5031,7 +5122,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -5039,7 +5130,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -5047,7 +5138,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="4">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -5071,7 +5162,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="4">
-        <v>1522</v>
+        <v>1523</v>
       </c>
     </row>
   </sheetData>
@@ -5114,7 +5205,7 @@
         <v>31</v>
       </c>
       <c r="B4" s="4">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -5122,7 +5213,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="4">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -5130,7 +5221,7 @@
         <v>33</v>
       </c>
       <c r="B6" s="4">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -5138,7 +5229,7 @@
         <v>34</v>
       </c>
       <c r="B7" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -5154,7 +5245,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="4">
-        <v>60</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -5164,15 +5255,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4396E4A6-D249-4F8F-BBB0-833858200275}">
-  <dimension ref="A2:B63"/>
+  <dimension ref="A2:B49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="69.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5194,7 +5285,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
@@ -5210,7 +5301,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>99</v>
+        <v>36</v>
       </c>
       <c r="B7" s="4">
         <v>2</v>
@@ -5218,23 +5309,23 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="B8" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="B9" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="B10" s="4">
         <v>1</v>
@@ -5242,15 +5333,15 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B11" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B12" s="4">
         <v>3</v>
@@ -5258,31 +5349,31 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="B14" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="B15" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" s="4">
         <v>1</v>
@@ -5290,15 +5381,15 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B17" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B18" s="4">
         <v>1</v>
@@ -5306,7 +5397,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B19" s="4">
         <v>1</v>
@@ -5314,7 +5405,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B20" s="4">
         <v>1</v>
@@ -5322,7 +5413,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B21" s="4">
         <v>1</v>
@@ -5330,31 +5421,31 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="B22" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="B23" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B24" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="B25" s="4">
         <v>2</v>
@@ -5362,39 +5453,39 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B26" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="B27" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B28" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="B29" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B30" s="4">
         <v>2</v>
@@ -5402,55 +5493,55 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B31" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="B32" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="B33" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B34" s="4">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="B35" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B36" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B37" s="4">
         <v>1</v>
@@ -5458,23 +5549,23 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="B38" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="B39" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="B40" s="4">
         <v>2</v>
@@ -5482,7 +5573,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B41" s="4">
         <v>1</v>
@@ -5490,15 +5581,15 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="B42" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="B43" s="4">
         <v>1</v>
@@ -5506,15 +5597,15 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="B44" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B45" s="4">
         <v>1</v>
@@ -5522,7 +5613,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B46" s="4">
         <v>1</v>
@@ -5530,138 +5621,26 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="B47" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="B48" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="B49" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B50" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B51" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B52" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B53" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B54" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B55" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B56" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B57" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B58" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B59" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B60" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B61" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B62" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B63" s="4">
-        <v>125</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -5673,8 +5652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68659609-96BE-43A8-866E-45E48E4CABC3}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5693,82 +5672,82 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B2" s="4">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B3" s="4">
-        <v>70</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B4" s="4">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B5" s="4">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B6" s="4">
-        <v>70</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B7" s="4">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B8" s="4">
-        <v>105</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B9" s="4">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B10" s="4">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B11" s="4">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -5776,7 +5755,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="4">
-        <v>535</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>